<commit_message>
Dorađen je Sprint BackLog, dodani su opisi i slike artefakata u tehničku dokumentaciju te su u projektnoj dokumentaciji dodani opisi održanih sastanaka, kao i slika burndown charta za prvi sprint.
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sprint BackLog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint BackLog'!$F$32:$H$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint BackLog'!$F$31:$H$40</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Zadatak</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Implementacija metoda za registraciju</t>
   </si>
   <si>
-    <t>Testiranje fukcionalnosti</t>
-  </si>
-  <si>
     <t>Izrada dijagrama klasa</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>Domagoj</t>
   </si>
   <si>
-    <t>Antonio,Andrea,Domagoj,Marijan</t>
-  </si>
-  <si>
     <t>Broj sati</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>19.10.2017.</t>
   </si>
   <si>
-    <t>02.11.2017.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Završetak </t>
   </si>
   <si>
@@ -153,6 +144,36 @@
   </si>
   <si>
     <t>Preostali napor</t>
+  </si>
+  <si>
+    <t>19.10.</t>
+  </si>
+  <si>
+    <t>25.10.</t>
+  </si>
+  <si>
+    <t>26.10.</t>
+  </si>
+  <si>
+    <t>31.10.2017.</t>
+  </si>
+  <si>
+    <t>31.10.</t>
+  </si>
+  <si>
+    <t>28.10.</t>
+  </si>
+  <si>
+    <t>29.10.</t>
+  </si>
+  <si>
+    <t>22.10.</t>
+  </si>
+  <si>
+    <t>24.10.</t>
+  </si>
+  <si>
+    <t>30.10.</t>
   </si>
 </sst>
 </file>
@@ -229,12 +250,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -245,8 +260,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -304,25 +325,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -339,26 +379,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,6 +395,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,8 +535,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.7136482939632549E-2"/>
-          <c:y val="0.17634259259259263"/>
+          <c:x val="5.2692038495188109E-2"/>
+          <c:y val="0.16245370370370371"/>
           <c:w val="0.90286351706036749"/>
           <c:h val="0.61498432487605714"/>
         </c:manualLayout>
@@ -486,16 +560,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint BackLog'!$G$2:$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>19.10.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.10.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.10.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.10.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.10.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.10.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.10.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.10.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.10.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint BackLog'!$F$33:$F$41</c:f>
+              <c:f>'Sprint BackLog'!$F$32:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -521,37 +642,84 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint BackLog'!$G$2:$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>19.10.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.10.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.10.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.10.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.10.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.10.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.10.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.10.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.10.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint BackLog'!$G$33:$G$41</c:f>
+              <c:f>'Sprint BackLog'!$G$32:$G$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -569,17 +737,19 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1249549632"/>
-        <c:axId val="-1249549088"/>
+        <c:axId val="1433651520"/>
+        <c:axId val="1433652608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1249549632"/>
+        <c:axId val="1433651520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -616,7 +786,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249549088"/>
+        <c:crossAx val="1433652608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -624,7 +794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1249549088"/>
+        <c:axId val="1433652608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,7 +845,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1249549632"/>
+        <c:crossAx val="1433651520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -797,7 +967,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -905,11 +1075,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -920,11 +1085,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -956,9 +1116,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1316,16 +1473,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1610,10 +1767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:O41"/>
+  <dimension ref="C2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,699 +1779,808 @@
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="14" max="15" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="3" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6">
+      <c r="D4" s="15"/>
+      <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="J4" s="20">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2">
+        <v>3</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="21">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6" s="21">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2">
         <v>3</v>
       </c>
-      <c r="H4" s="6">
-        <v>2</v>
-      </c>
-      <c r="I4" s="6">
+      <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="I8" s="21">
         <v>0</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2">
+        <v>4</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="21">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2">
+        <v>4</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="15">
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>3</v>
+      </c>
+      <c r="N11" s="2">
+        <v>2</v>
+      </c>
+      <c r="O11" s="21">
         <v>0</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6" t="s">
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5</v>
+      </c>
+      <c r="L12" s="2">
+        <v>5</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4</v>
+      </c>
+      <c r="N12" s="2">
+        <v>2</v>
+      </c>
+      <c r="O12" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="2">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2">
+        <v>4</v>
+      </c>
+      <c r="J13" s="2">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2">
+        <v>4</v>
+      </c>
+      <c r="L13" s="2">
+        <v>3</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>2</v>
+      </c>
+      <c r="M14" s="2">
+        <v>2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>2</v>
+      </c>
+      <c r="O14" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2</v>
+      </c>
+      <c r="L15" s="2">
+        <v>2</v>
+      </c>
+      <c r="M15" s="2">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>2</v>
+      </c>
+      <c r="O15" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="2">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="15">
+      <c r="G16" s="2">
+        <v>6</v>
+      </c>
+      <c r="H16" s="2">
+        <v>6</v>
+      </c>
+      <c r="I16" s="2">
+        <v>6</v>
+      </c>
+      <c r="J16" s="2">
+        <v>6</v>
+      </c>
+      <c r="K16" s="2">
+        <v>5</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3</v>
+      </c>
+      <c r="M16" s="21">
         <v>0</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="15">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6">
-        <v>5</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="6">
-        <v>3</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-      <c r="I8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6">
-        <v>4</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6">
-        <v>2</v>
-      </c>
-      <c r="J9" s="15">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6">
-        <v>4</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6">
-        <v>2</v>
-      </c>
-      <c r="J10" s="15">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6">
-        <v>5</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6">
-        <v>3</v>
-      </c>
-      <c r="N11" s="6">
-        <v>2</v>
-      </c>
-      <c r="O11" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6">
-        <v>5</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6">
-        <v>4</v>
-      </c>
-      <c r="L12" s="6">
-        <v>2</v>
-      </c>
-      <c r="M12" s="15">
-        <v>0</v>
-      </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6">
-        <v>4</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6">
-        <v>3</v>
-      </c>
-      <c r="M13" s="6">
-        <v>3</v>
-      </c>
-      <c r="N13" s="15">
-        <v>0</v>
-      </c>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6">
-        <v>3</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6">
-        <v>2</v>
-      </c>
-      <c r="N14" s="6">
-        <v>1</v>
-      </c>
-      <c r="O14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6">
-        <v>2</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="15">
-        <v>0</v>
-      </c>
-      <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6">
-        <v>2</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6">
-        <v>1</v>
-      </c>
-      <c r="N16" s="15">
-        <v>0</v>
-      </c>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+      <c r="D17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6">
-        <v>6</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="E17" s="8">
+        <f>SUM(E4:E16)</f>
+        <v>46</v>
+      </c>
+      <c r="F17" s="17"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="6">
-        <v>5</v>
-      </c>
-      <c r="L17" s="6">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="7"/>
+      <c r="D18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="8">
+        <v>2</v>
+      </c>
+      <c r="H18" s="8">
+        <v>4</v>
+      </c>
+      <c r="I18" s="8">
         <v>3</v>
       </c>
-      <c r="M17" s="6">
-        <v>2</v>
-      </c>
-      <c r="N17" s="15">
+      <c r="J18" s="8">
+        <v>4</v>
+      </c>
+      <c r="K18" s="8">
+        <v>3</v>
+      </c>
+      <c r="L18" s="8">
+        <v>7</v>
+      </c>
+      <c r="M18" s="8">
+        <v>10</v>
+      </c>
+      <c r="N18" s="8">
+        <v>6</v>
+      </c>
+      <c r="O18" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="8">
+        <v>46</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="8">
+        <f>E19-G18</f>
+        <v>44</v>
+      </c>
+      <c r="H19" s="8">
+        <f>G19-H18</f>
+        <v>40</v>
+      </c>
+      <c r="I19" s="8">
+        <f t="shared" ref="I19:M19" si="0">H19-I18</f>
+        <v>37</v>
+      </c>
+      <c r="J19" s="8">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K19" s="8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L19" s="8">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="M19" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="N19" s="8">
+        <f>M19-N18</f>
+        <v>7</v>
+      </c>
+      <c r="O19" s="8">
+        <f>N19-O18</f>
         <v>0</v>
       </c>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="11"/>
-      <c r="D18" s="9" t="s">
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="13">
-        <f>SUM(E4:E17)</f>
-        <v>49</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-    </row>
-    <row r="19" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="11"/>
-      <c r="D19" s="9" t="s">
+      <c r="E22" s="4">
+        <f>SUM(E4+E9+E10)</f>
+        <v>12</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4">
+        <f>SUM(E5+E7+E12+E13+E15)</f>
+        <v>14</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16">
+        <v>9</v>
+      </c>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="4">
+        <f>SUM(E8+E16)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="4">
+        <f>SUM(E6+E11+E14)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="9">
+        <f>SUM(E22:E25)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D28" s="10"/>
+    </row>
+    <row r="31" spans="3:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F31" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="13">
-        <v>4</v>
-      </c>
-      <c r="H19" s="13">
-        <v>5</v>
-      </c>
-      <c r="I19" s="13">
-        <v>6</v>
-      </c>
-      <c r="J19" s="13">
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="F32" s="2">
+        <v>46</v>
+      </c>
+      <c r="G32" s="12">
+        <f>F32-G18</f>
+        <v>44</v>
+      </c>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="2"/>
+      <c r="G33" s="12">
+        <f>G32-H18</f>
+        <v>40</v>
+      </c>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F34" s="2"/>
+      <c r="G34" s="12">
+        <f>G33-I18</f>
+        <v>37</v>
+      </c>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="2"/>
+      <c r="G35" s="12">
+        <f>G34-J18</f>
+        <v>33</v>
+      </c>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="2"/>
+      <c r="G36" s="12">
+        <f>G35-K18</f>
+        <v>30</v>
+      </c>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="2"/>
+      <c r="G37" s="12">
+        <f>G36-L18</f>
+        <v>23</v>
+      </c>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F38" s="2"/>
+      <c r="G38" s="12">
+        <f>G37-M18</f>
+        <v>13</v>
+      </c>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F39" s="2"/>
+      <c r="G39" s="12">
+        <f>G38-N18</f>
         <v>7</v>
       </c>
-      <c r="K19" s="13">
-        <v>2</v>
-      </c>
-      <c r="L19" s="13">
-        <v>5</v>
-      </c>
-      <c r="M19" s="13">
-        <v>7</v>
-      </c>
-      <c r="N19" s="13">
-        <v>10</v>
-      </c>
-      <c r="O19" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="13">
-        <v>49</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="13">
-        <f>E20-G19</f>
-        <v>45</v>
-      </c>
-      <c r="H20" s="13">
-        <f>G20-H19</f>
-        <v>40</v>
-      </c>
-      <c r="I20" s="13">
-        <f>H20-I19</f>
-        <v>34</v>
-      </c>
-      <c r="J20" s="13">
-        <f>I20-J19</f>
-        <v>27</v>
-      </c>
-      <c r="K20" s="13">
-        <f>J20-K19</f>
-        <v>25</v>
-      </c>
-      <c r="L20" s="13">
-        <f>K20-L19</f>
-        <v>20</v>
-      </c>
-      <c r="M20" s="13">
-        <f>L20-M19</f>
-        <v>13</v>
-      </c>
-      <c r="N20" s="13">
-        <f>M20-N19</f>
-        <v>3</v>
-      </c>
-      <c r="O20" s="13">
-        <f>N20-O19</f>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F40" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="E22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="8">
-        <f>SUM(E4+E9+E14+E10)</f>
-        <v>15</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="8">
-        <f>SUM(E5+E7+E12+E13+E16+E14)</f>
-        <v>17</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12">
-        <v>9</v>
-      </c>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="8">
-        <f>SUM(E8+E17+E14)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="8">
-        <f>SUM(E6+E11+E14+E15)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D27" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="16">
-        <f>SUM(E23:E26)</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D29" s="17"/>
-    </row>
-    <row r="32" spans="3:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F32" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="H32" s="19"/>
-    </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F33" s="6">
-        <v>49</v>
-      </c>
-      <c r="G33" s="20">
-        <f>F33-G19</f>
-        <v>45</v>
-      </c>
-      <c r="H33" s="21"/>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F34" s="6"/>
-      <c r="G34" s="20">
-        <f>G33-H19</f>
-        <v>40</v>
-      </c>
-      <c r="H34" s="21"/>
-    </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F35" s="6"/>
-      <c r="G35" s="20">
-        <f>G34-I19</f>
-        <v>34</v>
-      </c>
-      <c r="H35" s="21"/>
-    </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F36" s="6"/>
-      <c r="G36" s="20">
-        <f>G35-J19</f>
-        <v>27</v>
-      </c>
-      <c r="H36" s="21"/>
-    </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F37" s="6"/>
-      <c r="G37" s="20">
-        <f>G36-K19</f>
-        <v>25</v>
-      </c>
-      <c r="H37" s="21"/>
-    </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F38" s="6"/>
-      <c r="G38" s="20">
-        <f>G37-L19</f>
-        <v>20</v>
-      </c>
-      <c r="H38" s="21"/>
-    </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F39" s="6"/>
-      <c r="G39" s="20">
-        <f>G38-M19</f>
-        <v>13</v>
-      </c>
-      <c r="H39" s="21"/>
-    </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F40" s="6"/>
-      <c r="G40" s="20">
-        <f>G39-N19</f>
-        <v>3</v>
-      </c>
-      <c r="H40" s="21"/>
-    </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F41" s="6">
+      <c r="G40" s="12">
+        <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="G41" s="20">
-        <f>G40-O19</f>
-        <v>0</v>
-      </c>
-      <c r="H41" s="21"/>
+      <c r="H40" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="F32:H41">
+  <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
-  <mergeCells count="32">
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
+  <mergeCells count="34">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G20:O20"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
@@ -2323,6 +2589,28 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Popravljen je SprintBacklog iz prvog sprinta te su sada zadaci grupirani po funkcionalnostima.
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>Zadatak</t>
   </si>
@@ -174,13 +174,22 @@
   </si>
   <si>
     <t>30.10.</t>
+  </si>
+  <si>
+    <t>Registracija</t>
+  </si>
+  <si>
+    <t>Prijava</t>
+  </si>
+  <si>
+    <t>Bar-code čitač</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +225,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +283,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -346,7 +369,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -360,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -389,6 +438,49 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -398,49 +490,20 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,7 +761,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>40</c:v>
@@ -719,7 +782,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -739,11 +802,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1433651520"/>
-        <c:axId val="1433652608"/>
+        <c:axId val="-2102730832"/>
+        <c:axId val="-2102743888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1433651520"/>
+        <c:axId val="-2102730832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +849,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1433652608"/>
+        <c:crossAx val="-2102743888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -794,7 +857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1433652608"/>
+        <c:axId val="-2102743888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +908,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1433651520"/>
+        <c:crossAx val="-2102730832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1473,16 +1536,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>294217</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>603250</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1767,59 +1830,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O40"/>
+  <dimension ref="B1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
     <col min="14" max="15" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="22" t="s">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+    </row>
+    <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O2" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="30"/>
+      <c r="C3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -1854,11 +1935,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="15" t="s">
+    <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="31"/>
+      <c r="C4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="2">
         <v>4</v>
       </c>
@@ -1874,7 +1956,7 @@
       <c r="I4" s="2">
         <v>4</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="13">
         <v>4</v>
       </c>
       <c r="K4" s="2">
@@ -1886,16 +1968,17 @@
       <c r="M4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="14">
         <v>0</v>
       </c>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="15" t="s">
+    <row r="5" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="31"/>
+      <c r="C5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="2">
         <v>2</v>
       </c>
@@ -1917,18 +2000,21 @@
       <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="14">
         <v>0</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="15" t="s">
+    <row r="6" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -1950,18 +2036,19 @@
       <c r="K6" s="2">
         <v>2</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="14">
         <v>0</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="15" t="s">
+    <row r="7" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="31"/>
+      <c r="C7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -1971,7 +2058,7 @@
       <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="14">
         <v>0</v>
       </c>
       <c r="I7" s="2"/>
@@ -1982,11 +2069,12 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+    <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="31"/>
+      <c r="C8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="22"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -1999,7 +2087,7 @@
       <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
       <c r="J8" s="2"/>
@@ -2009,11 +2097,12 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="15"/>
+    <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="22"/>
       <c r="E9" s="2">
         <v>4</v>
       </c>
@@ -2027,275 +2116,287 @@
         <v>4</v>
       </c>
       <c r="I9" s="2">
-        <v>2</v>
-      </c>
-      <c r="J9" s="21">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="14">
         <v>0</v>
       </c>
-      <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="15"/>
+    <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
+      <c r="C10" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="22"/>
       <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5</v>
+      </c>
+      <c r="L10" s="2">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="2">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2">
-        <v>4</v>
-      </c>
-      <c r="I10" s="2">
-        <v>4</v>
-      </c>
-      <c r="J10" s="2">
-        <v>2</v>
-      </c>
-      <c r="K10" s="21">
+      <c r="N10" s="2">
+        <v>2</v>
+      </c>
+      <c r="O10" s="14">
         <v>0</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="15"/>
+    </row>
+    <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
+      <c r="C11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="22"/>
       <c r="E11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L11" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N11" s="2">
         <v>2</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="15"/>
+    <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
+      <c r="C12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="22"/>
       <c r="E12" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>2</v>
+      </c>
+      <c r="M12" s="2">
+        <v>2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>2</v>
+      </c>
+      <c r="O12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="33"/>
+      <c r="C13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="2">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2">
+        <v>6</v>
+      </c>
+      <c r="H13" s="2">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6</v>
+      </c>
+      <c r="J13" s="2">
+        <v>6</v>
+      </c>
+      <c r="K13" s="2">
         <v>5</v>
-      </c>
-      <c r="H12" s="2">
-        <v>5</v>
-      </c>
-      <c r="I12" s="2">
-        <v>5</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5</v>
-      </c>
-      <c r="K12" s="2">
-        <v>5</v>
-      </c>
-      <c r="L12" s="2">
-        <v>5</v>
-      </c>
-      <c r="M12" s="2">
-        <v>4</v>
-      </c>
-      <c r="N12" s="2">
-        <v>2</v>
-      </c>
-      <c r="O12" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="2">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="2">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2">
-        <v>4</v>
-      </c>
-      <c r="I13" s="2">
-        <v>4</v>
-      </c>
-      <c r="J13" s="2">
-        <v>4</v>
-      </c>
-      <c r="K13" s="2">
-        <v>4</v>
       </c>
       <c r="L13" s="2">
         <v>3</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="14">
         <v>0</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="2">
-        <v>2</v>
-      </c>
-      <c r="F14" s="2" t="s">
+    <row r="14" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="12">
+        <v>4</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="12">
+        <v>4</v>
+      </c>
+      <c r="H14" s="12">
+        <v>4</v>
+      </c>
+      <c r="I14" s="12">
+        <v>2</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="34"/>
+      <c r="C15" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="12">
+        <v>5</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="2">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2</v>
-      </c>
-      <c r="I14" s="2">
-        <v>2</v>
-      </c>
-      <c r="J14" s="2">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2">
-        <v>2</v>
-      </c>
-      <c r="L14" s="2">
-        <v>2</v>
-      </c>
-      <c r="M14" s="2">
-        <v>2</v>
-      </c>
-      <c r="N14" s="2">
-        <v>2</v>
-      </c>
-      <c r="O14" s="21">
+      <c r="G15" s="12">
+        <v>5</v>
+      </c>
+      <c r="H15" s="12">
+        <v>5</v>
+      </c>
+      <c r="I15" s="12">
+        <v>5</v>
+      </c>
+      <c r="J15" s="12">
+        <v>5</v>
+      </c>
+      <c r="K15" s="12">
+        <v>5</v>
+      </c>
+      <c r="L15" s="12">
+        <v>5</v>
+      </c>
+      <c r="M15" s="12">
+        <v>3</v>
+      </c>
+      <c r="N15" s="12">
+        <v>2</v>
+      </c>
+      <c r="O15" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2" t="s">
+    <row r="16" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="12">
+        <v>4</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="2">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2">
-        <v>2</v>
-      </c>
-      <c r="I15" s="2">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2</v>
-      </c>
-      <c r="L15" s="2">
-        <v>2</v>
-      </c>
-      <c r="M15" s="2">
-        <v>2</v>
-      </c>
-      <c r="N15" s="2">
-        <v>2</v>
-      </c>
-      <c r="O15" s="21">
+      <c r="G16" s="12">
+        <v>4</v>
+      </c>
+      <c r="H16" s="12">
+        <v>4</v>
+      </c>
+      <c r="I16" s="12">
+        <v>4</v>
+      </c>
+      <c r="J16" s="12">
+        <v>4</v>
+      </c>
+      <c r="K16" s="12">
+        <v>4</v>
+      </c>
+      <c r="L16" s="12">
+        <v>3</v>
+      </c>
+      <c r="M16" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="2">
-        <v>6</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="2">
-        <v>6</v>
-      </c>
-      <c r="H16" s="2">
-        <v>6</v>
-      </c>
-      <c r="I16" s="2">
-        <v>6</v>
-      </c>
-      <c r="J16" s="2">
-        <v>6</v>
-      </c>
-      <c r="K16" s="2">
-        <v>5</v>
-      </c>
-      <c r="L16" s="2">
-        <v>3</v>
-      </c>
-      <c r="M16" s="21">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="25"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -2304,7 +2405,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2315,18 +2416,19 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="21"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="28"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="8">
         <v>3</v>
@@ -2344,13 +2446,14 @@
         <v>10</v>
       </c>
       <c r="N18" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O18" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="21"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -2358,10 +2461,10 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="28"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H19" s="8">
         <f>G19-H18</f>
@@ -2389,93 +2492,93 @@
       </c>
       <c r="N19" s="8">
         <f>M19-N18</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O19" s="8">
         <f>N19-O18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16" t="s">
+      <c r="H21" s="24"/>
+      <c r="I21" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J21" s="24"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="4">
-        <f>SUM(E4+E9+E10)</f>
+        <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16" t="s">
+      <c r="H22" s="24"/>
+      <c r="I22" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J22" s="24"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="4">
-        <f>SUM(E5+E7+E12+E13+E15)</f>
+        <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16">
+      <c r="H23" s="24"/>
+      <c r="I23" s="24">
         <v>9</v>
       </c>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J23" s="24"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="4">
-        <f>SUM(E8+E16)</f>
+        <f>SUM(E8+E13)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D25" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="4">
-        <f>SUM(E6+E11+E14)</f>
+        <f>SUM(E6+E11+E15)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="3:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26" s="9" t="s">
         <v>23</v>
       </c>
@@ -2484,123 +2587,110 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D28" s="10"/>
     </row>
-    <row r="31" spans="3:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="14"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="H31" s="29"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="27">
         <f>F32-G18</f>
-        <v>44</v>
-      </c>
-      <c r="H32" s="13"/>
+        <v>43</v>
+      </c>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="12">
+      <c r="G33" s="27">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="13"/>
+      <c r="H33" s="28"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="12">
+      <c r="G34" s="27">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="13"/>
+      <c r="H34" s="28"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="12">
+      <c r="G35" s="27">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="13"/>
+      <c r="H35" s="28"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="12">
+      <c r="G36" s="27">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="13"/>
+      <c r="H36" s="28"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="12">
+      <c r="G37" s="27">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="13"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="12">
+      <c r="G38" s="27">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="13"/>
+      <c r="H38" s="28"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="12">
+      <c r="G39" s="27">
         <f>G38-N18</f>
-        <v>7</v>
-      </c>
-      <c r="H39" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="H39" s="28"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="27">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="13"/>
+      <c r="H40" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
-  <mergeCells count="34">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G20:O20"/>
-    <mergeCell ref="D20:E20"/>
+  <mergeCells count="36">
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
     <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="F17:F19"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="G39:H39"/>
@@ -2611,6 +2701,21 @@
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G20:O20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Dodane je opis retrospektivnog sastanka te je u excelu kreiran sprintbacklog za drugi sprint kojeg će trebati još doraditi.
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint BackLog" sheetId="1" r:id="rId1"/>
+    <sheet name="SprintBackLog 1" sheetId="1" r:id="rId1"/>
+    <sheet name="SpirntBacklog 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint BackLog'!$F$31:$H$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SpirntBacklog 2'!$E$39:$F$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SprintBackLog 1'!$F$31:$H$40</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>Zadatak</t>
   </si>
@@ -183,13 +185,106 @@
   </si>
   <si>
     <t>Bar-code čitač</t>
+  </si>
+  <si>
+    <t>Popis lijekova</t>
+  </si>
+  <si>
+    <t>Implementirati dva načina prikaza lijekova</t>
+  </si>
+  <si>
+    <t>Implementirati modularnost</t>
+  </si>
+  <si>
+    <t>26.11.2017.</t>
+  </si>
+  <si>
+    <t>28.11.2017.</t>
+  </si>
+  <si>
+    <t>29.11.2017.</t>
+  </si>
+  <si>
+    <t>01.12.2017.</t>
+  </si>
+  <si>
+    <t>03.12.2017.</t>
+  </si>
+  <si>
+    <t>07.12.2017.</t>
+  </si>
+  <si>
+    <t>08.12.2017.</t>
+  </si>
+  <si>
+    <t>06.12.2017.</t>
+  </si>
+  <si>
+    <t>Izraditi listu pregleda korisnika</t>
+  </si>
+  <si>
+    <t>Izraditi aktivnost za unos podataka o novom pregledu</t>
+  </si>
+  <si>
+    <t>Implementirati metode za dodavanje novog pregleda</t>
+  </si>
+  <si>
+    <t>Izraditi dijagram klasa</t>
+  </si>
+  <si>
+    <t>Izrada aktivnosti za izmjenu podataka</t>
+  </si>
+  <si>
+    <t>Implementirati metode za izmjenu podataka</t>
+  </si>
+  <si>
+    <t>Izmjena korisničkih podataka</t>
+  </si>
+  <si>
+    <t>Unos terapije</t>
+  </si>
+  <si>
+    <t>Prikaz pregleda</t>
+  </si>
+  <si>
+    <t>Unos novog pregleda</t>
+  </si>
+  <si>
+    <t>Pokretanje/Zaustavljanje terapije</t>
+  </si>
+  <si>
+    <t>Izraditi aktivnost za unos nove terapije</t>
+  </si>
+  <si>
+    <t>Implementirati metode za unos nove terapije</t>
+  </si>
+  <si>
+    <t>Izraditi aktivnost za pokretanje/zaustavljanje terapije</t>
+  </si>
+  <si>
+    <t>Implementirati metode za pokretanje/zaustavljanje terapije</t>
+  </si>
+  <si>
+    <t>05.12.2017.</t>
+  </si>
+  <si>
+    <t>09.12.2017.</t>
+  </si>
+  <si>
+    <t>15.11.2017.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dan 9 </t>
+  </si>
+  <si>
+    <t>Dan 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +328,16 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +389,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,24 +587,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,9 +600,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -502,6 +614,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -639,7 +823,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint BackLog'!$G$2:$O$2</c:f>
+              <c:f>'SprintBackLog 1'!$G$2:$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -674,7 +858,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint BackLog'!$F$32:$F$40</c:f>
+              <c:f>'SprintBackLog 1'!$F$32:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -721,7 +905,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint BackLog'!$G$2:$O$2</c:f>
+              <c:f>'SprintBackLog 1'!$G$2:$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -756,7 +940,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint BackLog'!$G$32:$G$40</c:f>
+              <c:f>'SprintBackLog 1'!$G$32:$G$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -802,11 +986,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2102730832"/>
-        <c:axId val="-2102743888"/>
+        <c:axId val="-1833997632"/>
+        <c:axId val="-1834001984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2102730832"/>
+        <c:axId val="-1833997632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +1033,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102743888"/>
+        <c:crossAx val="-1834001984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -857,7 +1041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2102743888"/>
+        <c:axId val="-1834001984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,7 +1092,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102730832"/>
+        <c:crossAx val="-1833997632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -962,9 +1146,8 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="accent1">
+          <a:alpha val="98000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -1832,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView topLeftCell="F10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,27 +2029,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
@@ -1896,11 +2079,11 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30"/>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -1936,11 +2119,11 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="31"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="2">
         <v>4</v>
       </c>
@@ -1974,11 +2157,11 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="2">
         <v>2</v>
       </c>
@@ -2008,13 +2191,13 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -2044,11 +2227,11 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="31"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -2070,11 +2253,11 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -2098,11 +2281,11 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="22" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="2">
         <v>4</v>
       </c>
@@ -2130,11 +2313,11 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="2">
         <v>5</v>
       </c>
@@ -2170,11 +2353,11 @@
       </c>
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="2">
         <v>2</v>
       </c>
@@ -2210,11 +2393,11 @@
       </c>
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="2">
         <v>2</v>
       </c>
@@ -2250,11 +2433,11 @@
       </c>
     </row>
     <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="2">
         <v>6</v>
       </c>
@@ -2286,13 +2469,13 @@
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="12">
         <v>4</v>
       </c>
@@ -2318,11 +2501,11 @@
       <c r="O14" s="12"/>
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="34"/>
-      <c r="C15" s="27" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="12">
         <v>5</v>
       </c>
@@ -2358,13 +2541,13 @@
       </c>
     </row>
     <row r="16" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="12">
         <v>4</v>
       </c>
@@ -2396,7 +2579,7 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="25"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -2405,7 +2588,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2417,13 +2600,13 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="26"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="8">
         <v>3</v>
       </c>
@@ -2453,7 +2636,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -2461,7 +2644,7 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="26"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
         <v>43</v>
@@ -2483,7 +2666,7 @@
         <v>30</v>
       </c>
       <c r="L19" s="8">
-        <f t="shared" si="0"/>
+        <f>K19-L18</f>
         <v>23</v>
       </c>
       <c r="M19" s="8">
@@ -2500,31 +2683,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24" t="s">
+      <c r="H21" s="37"/>
+      <c r="I21" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="37"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
@@ -2534,14 +2717,14 @@
         <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24" t="s">
+      <c r="H22" s="37"/>
+      <c r="I22" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="24"/>
+      <c r="J22" s="37"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
@@ -2551,14 +2734,14 @@
         <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24">
+      <c r="H23" s="37"/>
+      <c r="I23" s="37">
         <v>9</v>
       </c>
-      <c r="J23" s="24"/>
+      <c r="J23" s="37"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -2594,116 +2777,92 @@
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="29" t="s">
+      <c r="G31" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="29"/>
+      <c r="H31" s="38"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="27">
+      <c r="G32" s="35">
         <f>F32-G18</f>
         <v>43</v>
       </c>
-      <c r="H32" s="28"/>
+      <c r="H32" s="36"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="27">
+      <c r="G33" s="35">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="28"/>
+      <c r="H33" s="36"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="27">
+      <c r="G34" s="35">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="28"/>
+      <c r="H34" s="36"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="27">
+      <c r="G35" s="35">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="28"/>
+      <c r="H35" s="36"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="27">
+      <c r="G36" s="35">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="28"/>
+      <c r="H36" s="36"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="27">
+      <c r="G37" s="35">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="28"/>
+      <c r="H37" s="36"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="27">
+      <c r="G38" s="35">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="28"/>
+      <c r="H38" s="36"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="27">
+      <c r="G39" s="35">
         <f>G38-N18</f>
         <v>8</v>
       </c>
-      <c r="H39" s="28"/>
+      <c r="H39" s="36"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G40" s="35">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="28"/>
+      <c r="H40" s="36"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="36">
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C16:D16"/>
     <mergeCell ref="G20:O20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C12:D12"/>
@@ -2716,9 +2875,1068 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:Q49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="1.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="49.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="22"/>
+    </row>
+    <row r="4" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="25"/>
+      <c r="D5" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="26"/>
+      <c r="D6" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="20">
+        <v>9</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="20">
+        <v>9</v>
+      </c>
+      <c r="I6" s="20">
+        <v>9</v>
+      </c>
+      <c r="J6" s="20">
+        <v>9</v>
+      </c>
+      <c r="K6" s="13">
+        <v>9</v>
+      </c>
+      <c r="L6" s="20">
+        <v>9</v>
+      </c>
+      <c r="M6" s="20">
+        <v>4</v>
+      </c>
+      <c r="N6" s="49">
+        <v>0</v>
+      </c>
+      <c r="O6" s="20"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="48"/>
+    </row>
+    <row r="7" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="26"/>
+      <c r="D7" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="20">
+        <v>5</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="20">
+        <v>5</v>
+      </c>
+      <c r="I7" s="20">
+        <v>5</v>
+      </c>
+      <c r="J7" s="20">
+        <v>5</v>
+      </c>
+      <c r="K7" s="20">
+        <v>5</v>
+      </c>
+      <c r="L7" s="20">
+        <v>3</v>
+      </c>
+      <c r="M7" s="48">
+        <v>1</v>
+      </c>
+      <c r="N7" s="20">
+        <v>1</v>
+      </c>
+      <c r="O7" s="20">
+        <v>1</v>
+      </c>
+      <c r="P7" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="20"/>
+    </row>
+    <row r="8" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="34"/>
+      <c r="F8" s="20">
+        <v>2</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="20">
+        <v>2</v>
+      </c>
+      <c r="I8" s="20">
+        <v>2</v>
+      </c>
+      <c r="J8" s="20">
+        <v>2</v>
+      </c>
+      <c r="K8" s="20">
+        <v>2</v>
+      </c>
+      <c r="L8" s="20">
+        <v>2</v>
+      </c>
+      <c r="M8" s="48">
+        <v>2</v>
+      </c>
+      <c r="N8" s="20">
+        <v>2</v>
+      </c>
+      <c r="O8" s="20">
+        <v>2</v>
+      </c>
+      <c r="P8" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="20"/>
+    </row>
+    <row r="9" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="20">
+        <v>4</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="20">
+        <v>4</v>
+      </c>
+      <c r="I9" s="20">
+        <v>4</v>
+      </c>
+      <c r="J9" s="20">
+        <v>4</v>
+      </c>
+      <c r="K9" s="48">
+        <v>4</v>
+      </c>
+      <c r="L9" s="20">
+        <v>4</v>
+      </c>
+      <c r="M9" s="20">
+        <v>3</v>
+      </c>
+      <c r="N9" s="49">
+        <v>0</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="20"/>
+    </row>
+    <row r="10" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="20">
+        <v>4</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="20">
+        <v>4</v>
+      </c>
+      <c r="I10" s="20">
+        <v>4</v>
+      </c>
+      <c r="J10" s="20">
+        <v>4</v>
+      </c>
+      <c r="K10" s="20">
+        <v>4</v>
+      </c>
+      <c r="L10" s="20">
+        <v>4</v>
+      </c>
+      <c r="M10" s="20">
+        <v>4</v>
+      </c>
+      <c r="N10" s="20">
+        <v>2</v>
+      </c>
+      <c r="O10" s="20">
+        <v>2</v>
+      </c>
+      <c r="P10" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="20"/>
+    </row>
+    <row r="11" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="44"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="20">
+        <v>2</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="20">
+        <v>2</v>
+      </c>
+      <c r="I11" s="20">
+        <v>2</v>
+      </c>
+      <c r="J11" s="20">
+        <v>2</v>
+      </c>
+      <c r="K11" s="20">
+        <v>2</v>
+      </c>
+      <c r="L11" s="20">
+        <v>2</v>
+      </c>
+      <c r="M11" s="20">
+        <v>2</v>
+      </c>
+      <c r="N11" s="49">
+        <v>0</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="20"/>
+    </row>
+    <row r="12" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="43"/>
+      <c r="D12" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="20">
+        <v>2</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="20">
+        <v>2</v>
+      </c>
+      <c r="I12" s="20">
+        <v>2</v>
+      </c>
+      <c r="J12" s="20">
+        <v>2</v>
+      </c>
+      <c r="K12" s="20">
+        <v>2</v>
+      </c>
+      <c r="L12" s="20">
+        <v>2</v>
+      </c>
+      <c r="M12" s="20">
+        <v>2</v>
+      </c>
+      <c r="N12" s="20">
+        <v>2</v>
+      </c>
+      <c r="O12" s="20">
+        <v>2</v>
+      </c>
+      <c r="P12" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="20"/>
+    </row>
+    <row r="13" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="20">
+        <v>4</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="20">
+        <v>4</v>
+      </c>
+      <c r="I13" s="20">
+        <v>4</v>
+      </c>
+      <c r="J13" s="20">
+        <v>4</v>
+      </c>
+      <c r="K13" s="20">
+        <v>4</v>
+      </c>
+      <c r="L13" s="20">
+        <v>4</v>
+      </c>
+      <c r="M13" s="20">
+        <v>3</v>
+      </c>
+      <c r="N13" s="49">
+        <v>0</v>
+      </c>
+      <c r="O13" s="20"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="20"/>
+    </row>
+    <row r="14" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="44"/>
+      <c r="D14" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="20">
+        <v>6</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="20">
+        <v>6</v>
+      </c>
+      <c r="I14" s="20">
+        <v>6</v>
+      </c>
+      <c r="J14" s="20">
+        <v>6</v>
+      </c>
+      <c r="K14" s="20">
+        <v>6</v>
+      </c>
+      <c r="L14" s="20">
+        <v>6</v>
+      </c>
+      <c r="M14" s="20">
+        <v>6</v>
+      </c>
+      <c r="N14" s="20">
+        <v>4</v>
+      </c>
+      <c r="O14" s="20">
+        <v>3</v>
+      </c>
+      <c r="P14" s="46">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="43"/>
+      <c r="D15" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="20">
+        <v>2</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="20">
+        <v>2</v>
+      </c>
+      <c r="I15" s="20">
+        <v>2</v>
+      </c>
+      <c r="J15" s="20">
+        <v>2</v>
+      </c>
+      <c r="K15" s="20">
+        <v>2</v>
+      </c>
+      <c r="L15" s="20">
+        <v>2</v>
+      </c>
+      <c r="M15" s="20">
+        <v>2</v>
+      </c>
+      <c r="N15" s="20">
+        <v>2</v>
+      </c>
+      <c r="O15" s="20">
+        <v>2</v>
+      </c>
+      <c r="P15" s="46">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="26"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="20">
+        <v>3</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="20">
+        <v>3</v>
+      </c>
+      <c r="I16" s="20">
+        <v>3</v>
+      </c>
+      <c r="J16" s="20">
+        <v>3</v>
+      </c>
+      <c r="K16" s="20">
+        <v>3</v>
+      </c>
+      <c r="L16" s="20">
+        <v>3</v>
+      </c>
+      <c r="M16" s="20">
+        <v>3</v>
+      </c>
+      <c r="N16" s="20">
+        <v>3</v>
+      </c>
+      <c r="O16" s="20">
+        <v>1</v>
+      </c>
+      <c r="P16" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="20"/>
+    </row>
+    <row r="17" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="20">
+        <v>4</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="20">
+        <v>4</v>
+      </c>
+      <c r="I17" s="20">
+        <v>4</v>
+      </c>
+      <c r="J17" s="20">
+        <v>4</v>
+      </c>
+      <c r="K17" s="20">
+        <v>4</v>
+      </c>
+      <c r="L17" s="20">
+        <v>4</v>
+      </c>
+      <c r="M17" s="20">
+        <v>4</v>
+      </c>
+      <c r="N17" s="20">
+        <v>2</v>
+      </c>
+      <c r="O17" s="20">
+        <v>2</v>
+      </c>
+      <c r="P17" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="20"/>
+    </row>
+    <row r="18" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="20">
+        <v>5</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="20">
+        <v>5</v>
+      </c>
+      <c r="I18" s="20">
+        <v>5</v>
+      </c>
+      <c r="J18" s="20">
+        <v>5</v>
+      </c>
+      <c r="K18" s="20">
+        <v>5</v>
+      </c>
+      <c r="L18" s="20">
+        <v>3</v>
+      </c>
+      <c r="M18" s="49">
+        <v>0</v>
+      </c>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="20"/>
+    </row>
+    <row r="19" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="44"/>
+      <c r="D19" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="20">
+        <v>8</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="20">
+        <v>8</v>
+      </c>
+      <c r="I19" s="20">
+        <v>8</v>
+      </c>
+      <c r="J19" s="20">
+        <v>8</v>
+      </c>
+      <c r="K19" s="20">
+        <v>8</v>
+      </c>
+      <c r="L19" s="20">
+        <v>8</v>
+      </c>
+      <c r="M19" s="20">
+        <v>4</v>
+      </c>
+      <c r="N19" s="48">
+        <v>2</v>
+      </c>
+      <c r="O19" s="48">
+        <v>2</v>
+      </c>
+      <c r="P19" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="20"/>
+    </row>
+    <row r="20" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="43"/>
+      <c r="D20" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="20">
+        <v>2</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="20">
+        <v>2</v>
+      </c>
+      <c r="I20" s="20">
+        <v>2</v>
+      </c>
+      <c r="J20" s="20">
+        <v>2</v>
+      </c>
+      <c r="K20" s="20">
+        <v>2</v>
+      </c>
+      <c r="L20" s="20">
+        <v>2</v>
+      </c>
+      <c r="M20" s="20">
+        <v>2</v>
+      </c>
+      <c r="N20" s="48">
+        <v>2</v>
+      </c>
+      <c r="O20" s="48">
+        <v>2</v>
+      </c>
+      <c r="P20" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="20"/>
+    </row>
+    <row r="21" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C21" s="39"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="8">
+        <f>SUM(F6:F20)</f>
+        <v>62</v>
+      </c>
+      <c r="G21" s="39"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+    </row>
+    <row r="22" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="32"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0</v>
+      </c>
+      <c r="L22" s="8">
+        <v>4</v>
+      </c>
+      <c r="M22" s="8">
+        <v>16</v>
+      </c>
+      <c r="N22" s="8">
+        <v>20</v>
+      </c>
+      <c r="O22" s="8">
+        <v>3</v>
+      </c>
+      <c r="P22" s="8">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="8">
+        <f ca="1">P23-Q23</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="32"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="8">
+        <f>F21</f>
+        <v>62</v>
+      </c>
+      <c r="G23" s="39"/>
+      <c r="H23" s="8">
+        <f>F23-H22</f>
+        <v>62</v>
+      </c>
+      <c r="I23" s="8">
+        <f>H23-I22</f>
+        <v>62</v>
+      </c>
+      <c r="J23" s="8">
+        <f t="shared" ref="J23:N23" si="0">I23-J22</f>
+        <v>62</v>
+      </c>
+      <c r="K23" s="8">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="L23" s="8">
+        <f>K23-L22</f>
+        <v>58</v>
+      </c>
+      <c r="M23" s="8">
+        <f>L23-M22</f>
+        <v>42</v>
+      </c>
+      <c r="N23" s="8">
+        <f>M23-N22</f>
+        <v>22</v>
+      </c>
+      <c r="O23" s="8">
+        <f>N23-O22</f>
+        <v>19</v>
+      </c>
+      <c r="P23" s="8">
+        <f>O23-P22</f>
+        <v>3</v>
+      </c>
+      <c r="Q23" s="8">
+        <f ca="1">3-Q22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="F28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="L28" s="52"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="4">
+        <f>SUM(F18:F20)</f>
+        <v>15</v>
+      </c>
+      <c r="I29" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="L29" s="52"/>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="4">
+        <f>SUM(F6:F8)</f>
+        <v>16</v>
+      </c>
+      <c r="I30" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52">
+        <v>10</v>
+      </c>
+      <c r="L30" s="52"/>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="4">
+        <f>SUM(F9:F12)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="4">
+        <f>SUM(F13:F17)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="9">
+        <f>SUM(F29:F32)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E39" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E40" s="54">
+        <v>62</v>
+      </c>
+      <c r="F40" s="54">
+        <f>E40-H22</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E41" s="54"/>
+      <c r="F41" s="54">
+        <f>F40-I22</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E42" s="54"/>
+      <c r="F42" s="54">
+        <f>F41-J22</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E43" s="54"/>
+      <c r="F43" s="54">
+        <f>F42-K22</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E44" s="54"/>
+      <c r="F44" s="54">
+        <f>F43-L22</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E45" s="54"/>
+      <c r="F45" s="54">
+        <f>F44-M22</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E46" s="54"/>
+      <c r="F46" s="54">
+        <f>F45-N22</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E47" s="54"/>
+      <c r="F47" s="54">
+        <f>F46-O22</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E48" s="54"/>
+      <c r="F48" s="54">
+        <f>F47-P22</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E49" s="54">
+        <v>0</v>
+      </c>
+      <c r="F49" s="54">
+        <f ca="1">F48-Q22</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="E39:F49"/>
+  <mergeCells count="25">
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Omogućeno je kreiranje burndown charta za definirani sprint
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -616,49 +616,10 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,13 +640,52 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -986,11 +986,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1833997632"/>
-        <c:axId val="-1834001984"/>
+        <c:axId val="-852700128"/>
+        <c:axId val="-852127136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1833997632"/>
+        <c:axId val="-852700128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,7 +1033,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1834001984"/>
+        <c:crossAx val="-852127136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1041,7 +1041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1834001984"/>
+        <c:axId val="-852127136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1092,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1833997632"/>
+        <c:crossAx val="-852700128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1172,7 +1172,524 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>BurnDown chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sr-Latn-RS"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SpirntBacklog 2'!$E$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Idealno</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SpirntBacklog 2'!$H$4:$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>26.11.2017.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.11.2017.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.11.2017.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>01.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>03.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>05.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>06.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>07.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>08.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>09.12.2017.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SpirntBacklog 2'!$E$40:$E$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SpirntBacklog 2'!$F$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Preostali napor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SpirntBacklog 2'!$H$4:$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>26.11.2017.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.11.2017.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.11.2017.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>01.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>03.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>05.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>06.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>07.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>08.12.2017.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>09.12.2017.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SpirntBacklog 2'!$F$40:$F$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-333479568"/>
+        <c:axId val="-333478480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-333479568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sr-Latn-RS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-333478480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-333478480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sr-Latn-RS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-333479568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sr-Latn-RS"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sr-Latn-RS"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1715,6 +2232,508 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1733,6 +2752,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>188820</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>55227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>740709</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>167527</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2015,7 +3069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="F19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G20" sqref="G20:O20"/>
     </sheetView>
   </sheetViews>
@@ -2029,27 +3083,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
@@ -2080,10 +3134,10 @@
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -2120,10 +3174,10 @@
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="42"/>
       <c r="E4" s="2">
         <v>4</v>
       </c>
@@ -2158,10 +3212,10 @@
     </row>
     <row r="5" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26"/>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="2">
         <v>2</v>
       </c>
@@ -2194,10 +3248,10 @@
       <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="42"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -2228,10 +3282,10 @@
     </row>
     <row r="7" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26"/>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -2254,10 +3308,10 @@
     </row>
     <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26"/>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -2282,10 +3336,10 @@
     </row>
     <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="2">
         <v>4</v>
       </c>
@@ -2314,10 +3368,10 @@
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="2">
         <v>5</v>
       </c>
@@ -2354,10 +3408,10 @@
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="34"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="2">
         <v>2</v>
       </c>
@@ -2394,10 +3448,10 @@
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="2">
         <v>2</v>
       </c>
@@ -2434,10 +3488,10 @@
     </row>
     <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="34"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="2">
         <v>6</v>
       </c>
@@ -2472,10 +3526,10 @@
       <c r="B14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="12">
         <v>4</v>
       </c>
@@ -2502,10 +3556,10 @@
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29"/>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="12">
         <v>5</v>
       </c>
@@ -2544,10 +3598,10 @@
       <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="34"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="12">
         <v>4</v>
       </c>
@@ -2579,7 +3633,7 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -2588,7 +3642,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="31"/>
+      <c r="F17" s="48"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2600,13 +3654,13 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="39"/>
+      <c r="F18" s="50"/>
       <c r="G18" s="8">
         <v>3</v>
       </c>
@@ -2636,7 +3690,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="32"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -2644,7 +3698,7 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="39"/>
+      <c r="F19" s="50"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
         <v>43</v>
@@ -2683,31 +3737,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37" t="s">
+      <c r="H21" s="47"/>
+      <c r="I21" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="37"/>
+      <c r="J21" s="47"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
@@ -2717,14 +3771,14 @@
         <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37" t="s">
+      <c r="H22" s="47"/>
+      <c r="I22" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="37"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
@@ -2734,14 +3788,14 @@
         <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="37" t="s">
+      <c r="G23" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37">
+      <c r="H23" s="47"/>
+      <c r="I23" s="47">
         <v>9</v>
       </c>
-      <c r="J23" s="37"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -2777,92 +3831,116 @@
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="38" t="s">
+      <c r="G31" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="38"/>
+      <c r="H31" s="46"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="35">
+      <c r="G32" s="44">
         <f>F32-G18</f>
         <v>43</v>
       </c>
-      <c r="H32" s="36"/>
+      <c r="H32" s="45"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="35">
+      <c r="G33" s="44">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="36"/>
+      <c r="H33" s="45"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="35">
+      <c r="G34" s="44">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="36"/>
+      <c r="H34" s="45"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="35">
+      <c r="G35" s="44">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="36"/>
+      <c r="H35" s="45"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="35">
+      <c r="G36" s="44">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="36"/>
+      <c r="H36" s="45"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="35">
+      <c r="G37" s="44">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="36"/>
+      <c r="H37" s="45"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="35">
+      <c r="G38" s="44">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="36"/>
+      <c r="H38" s="45"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="35">
+      <c r="G39" s="44">
         <f>G38-N18</f>
         <v>8</v>
       </c>
-      <c r="H39" s="36"/>
+      <c r="H39" s="45"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="35">
+      <c r="G40" s="44">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="36"/>
+      <c r="H40" s="45"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="36">
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G20:O20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C12:D12"/>
@@ -2875,30 +3953,6 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2910,8 +3964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2932,29 +3986,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
       <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="41" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="31" t="s">
         <v>55</v>
       </c>
       <c r="I4" s="16" t="s">
@@ -2981,16 +4035,16 @@
       <c r="P4" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="Q4" s="42" t="s">
+      <c r="Q4" s="32" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="25"/>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="21" t="s">
         <v>34</v>
       </c>
@@ -3030,10 +4084,10 @@
     </row>
     <row r="6" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C6" s="26"/>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="20">
         <v>9</v>
       </c>
@@ -3058,19 +4112,19 @@
       <c r="M6" s="20">
         <v>4</v>
       </c>
-      <c r="N6" s="49">
+      <c r="N6" s="36">
         <v>0</v>
       </c>
       <c r="O6" s="20"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="48"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="35"/>
     </row>
     <row r="7" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C7" s="26"/>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="20">
         <v>5</v>
       </c>
@@ -3092,7 +4146,7 @@
       <c r="L7" s="20">
         <v>3</v>
       </c>
-      <c r="M7" s="48">
+      <c r="M7" s="35">
         <v>1</v>
       </c>
       <c r="N7" s="20">
@@ -3101,7 +4155,7 @@
       <c r="O7" s="20">
         <v>1</v>
       </c>
-      <c r="P7" s="50">
+      <c r="P7" s="37">
         <v>0</v>
       </c>
       <c r="Q7" s="20"/>
@@ -3110,10 +4164,10 @@
       <c r="C8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="20">
         <v>2</v>
       </c>
@@ -3135,7 +4189,7 @@
       <c r="L8" s="20">
         <v>2</v>
       </c>
-      <c r="M8" s="48">
+      <c r="M8" s="35">
         <v>2</v>
       </c>
       <c r="N8" s="20">
@@ -3144,7 +4198,7 @@
       <c r="O8" s="20">
         <v>2</v>
       </c>
-      <c r="P8" s="50">
+      <c r="P8" s="37">
         <v>0</v>
       </c>
       <c r="Q8" s="20"/>
@@ -3153,10 +4207,10 @@
       <c r="C9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="20">
         <v>4</v>
       </c>
@@ -3172,7 +4226,7 @@
       <c r="J9" s="20">
         <v>4</v>
       </c>
-      <c r="K9" s="48">
+      <c r="K9" s="35">
         <v>4</v>
       </c>
       <c r="L9" s="20">
@@ -3181,7 +4235,7 @@
       <c r="M9" s="20">
         <v>3</v>
       </c>
-      <c r="N9" s="49">
+      <c r="N9" s="36">
         <v>0</v>
       </c>
       <c r="O9" s="20"/>
@@ -3189,7 +4243,7 @@
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="52" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="23"/>
@@ -3226,13 +4280,13 @@
       <c r="O10" s="20">
         <v>2</v>
       </c>
-      <c r="P10" s="51">
+      <c r="P10" s="38">
         <v>0</v>
       </c>
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="44"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
         <v>64</v>
@@ -3261,19 +4315,19 @@
       <c r="M11" s="20">
         <v>2</v>
       </c>
-      <c r="N11" s="49">
+      <c r="N11" s="36">
         <v>0</v>
       </c>
       <c r="O11" s="20"/>
-      <c r="P11" s="46"/>
+      <c r="P11" s="33"/>
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="43"/>
-      <c r="D12" s="35" t="s">
+      <c r="C12" s="54"/>
+      <c r="D12" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="36"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="20">
         <v>2</v>
       </c>
@@ -3304,19 +4358,19 @@
       <c r="O12" s="20">
         <v>2</v>
       </c>
-      <c r="P12" s="51">
+      <c r="P12" s="38">
         <v>0</v>
       </c>
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="36"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="20">
         <v>4</v>
       </c>
@@ -3341,19 +4395,19 @@
       <c r="M13" s="20">
         <v>3</v>
       </c>
-      <c r="N13" s="49">
+      <c r="N13" s="36">
         <v>0</v>
       </c>
       <c r="O13" s="20"/>
-      <c r="P13" s="46"/>
+      <c r="P13" s="33"/>
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="44"/>
-      <c r="D14" s="35" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="36"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="20">
         <v>6</v>
       </c>
@@ -3384,19 +4438,19 @@
       <c r="O14" s="20">
         <v>3</v>
       </c>
-      <c r="P14" s="46">
+      <c r="P14" s="33">
         <v>1</v>
       </c>
-      <c r="Q14" s="49">
+      <c r="Q14" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="43"/>
-      <c r="D15" s="35" t="s">
+      <c r="C15" s="54"/>
+      <c r="D15" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="45"/>
       <c r="F15" s="20">
         <v>2</v>
       </c>
@@ -3427,10 +4481,10 @@
       <c r="O15" s="20">
         <v>2</v>
       </c>
-      <c r="P15" s="46">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="49">
+      <c r="P15" s="33">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="36">
         <v>0</v>
       </c>
     </row>
@@ -3470,7 +4524,7 @@
       <c r="O16" s="20">
         <v>1</v>
       </c>
-      <c r="P16" s="51">
+      <c r="P16" s="38">
         <v>0</v>
       </c>
       <c r="Q16" s="20"/>
@@ -3513,19 +4567,19 @@
       <c r="O17" s="20">
         <v>2</v>
       </c>
-      <c r="P17" s="51">
+      <c r="P17" s="38">
         <v>0</v>
       </c>
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="20">
         <v>5</v>
       </c>
@@ -3547,20 +4601,20 @@
       <c r="L18" s="20">
         <v>3</v>
       </c>
-      <c r="M18" s="49">
+      <c r="M18" s="36">
         <v>0</v>
       </c>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="46"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="33"/>
       <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="44"/>
-      <c r="D19" s="35" t="s">
+      <c r="C19" s="53"/>
+      <c r="D19" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="20">
         <v>8</v>
       </c>
@@ -3585,23 +4639,23 @@
       <c r="M19" s="20">
         <v>4</v>
       </c>
-      <c r="N19" s="48">
-        <v>2</v>
-      </c>
-      <c r="O19" s="48">
-        <v>2</v>
-      </c>
-      <c r="P19" s="49">
+      <c r="N19" s="35">
+        <v>2</v>
+      </c>
+      <c r="O19" s="35">
+        <v>2</v>
+      </c>
+      <c r="P19" s="36">
         <v>0</v>
       </c>
       <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="43"/>
-      <c r="D20" s="34" t="s">
+      <c r="C20" s="54"/>
+      <c r="D20" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="20">
         <v>2</v>
       </c>
@@ -3626,19 +4680,19 @@
       <c r="M20" s="20">
         <v>2</v>
       </c>
-      <c r="N20" s="48">
-        <v>2</v>
-      </c>
-      <c r="O20" s="48">
-        <v>2</v>
-      </c>
-      <c r="P20" s="49">
+      <c r="N20" s="35">
+        <v>2</v>
+      </c>
+      <c r="O20" s="35">
+        <v>2</v>
+      </c>
+      <c r="P20" s="36">
         <v>0</v>
       </c>
       <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="39"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
         <v>23</v>
@@ -3647,7 +4701,7 @@
         <f>SUM(F6:F20)</f>
         <v>62</v>
       </c>
-      <c r="G21" s="39"/>
+      <c r="G21" s="50"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -3660,13 +4714,13 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="32"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="39"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="8">
         <v>0</v>
       </c>
@@ -3695,12 +4749,12 @@
         <v>16</v>
       </c>
       <c r="Q22" s="8">
-        <f ca="1">P23-Q23</f>
+        <f>P23-Q23</f>
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="32"/>
+      <c r="C23" s="41"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>36</v>
@@ -3709,7 +4763,7 @@
         <f>F21</f>
         <v>62</v>
       </c>
-      <c r="G23" s="39"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="8">
         <f>F23-H22</f>
         <v>62</v>
@@ -3719,7 +4773,7 @@
         <v>62</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" ref="J23:N23" si="0">I23-J22</f>
+        <f t="shared" ref="J23:K23" si="0">I23-J22</f>
         <v>62</v>
       </c>
       <c r="K23" s="8">
@@ -3747,7 +4801,7 @@
         <v>3</v>
       </c>
       <c r="Q23" s="8">
-        <f ca="1">3-Q22</f>
+        <f>SUM(Q6:Q20)</f>
         <v>0</v>
       </c>
     </row>
@@ -3755,14 +4809,14 @@
       <c r="F28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="52" t="s">
+      <c r="I28" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52" t="s">
+      <c r="J28" s="51"/>
+      <c r="K28" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="L28" s="52"/>
+      <c r="L28" s="51"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E29" s="3" t="s">
@@ -3772,14 +4826,14 @@
         <f>SUM(F18:F20)</f>
         <v>15</v>
       </c>
-      <c r="I29" s="52" t="s">
+      <c r="I29" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52" t="s">
+      <c r="J29" s="51"/>
+      <c r="K29" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="52"/>
+      <c r="L29" s="51"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E30" s="3" t="s">
@@ -3789,14 +4843,14 @@
         <f>SUM(F6:F8)</f>
         <v>16</v>
       </c>
-      <c r="I30" s="52" t="s">
+      <c r="I30" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52">
+      <c r="J30" s="51"/>
+      <c r="K30" s="51">
         <v>10</v>
       </c>
-      <c r="L30" s="52"/>
+      <c r="L30" s="51"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
@@ -3826,101 +4880,96 @@
       </c>
     </row>
     <row r="39" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E39" s="53" t="s">
+      <c r="E39" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="53" t="s">
+      <c r="F39" s="39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E40" s="54">
+      <c r="E40" s="40">
         <v>62</v>
       </c>
-      <c r="F40" s="54">
+      <c r="F40" s="40">
         <f>E40-H22</f>
         <v>62</v>
       </c>
     </row>
     <row r="41" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E41" s="54"/>
-      <c r="F41" s="54">
+      <c r="E41" s="40"/>
+      <c r="F41" s="40">
         <f>F40-I22</f>
         <v>62</v>
       </c>
     </row>
     <row r="42" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E42" s="54"/>
-      <c r="F42" s="54">
+      <c r="E42" s="40"/>
+      <c r="F42" s="40">
         <f>F41-J22</f>
         <v>62</v>
       </c>
     </row>
     <row r="43" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E43" s="54"/>
-      <c r="F43" s="54">
+      <c r="E43" s="40"/>
+      <c r="F43" s="40">
         <f>F42-K22</f>
         <v>62</v>
       </c>
     </row>
     <row r="44" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E44" s="54"/>
-      <c r="F44" s="54">
+      <c r="E44" s="40"/>
+      <c r="F44" s="40">
         <f>F43-L22</f>
         <v>58</v>
       </c>
     </row>
     <row r="45" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E45" s="54"/>
-      <c r="F45" s="54">
+      <c r="E45" s="40"/>
+      <c r="F45" s="40">
         <f>F44-M22</f>
         <v>42</v>
       </c>
     </row>
     <row r="46" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E46" s="54"/>
-      <c r="F46" s="54">
+      <c r="E46" s="40"/>
+      <c r="F46" s="40">
         <f>F45-N22</f>
         <v>22</v>
       </c>
     </row>
     <row r="47" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E47" s="54"/>
-      <c r="F47" s="54">
+      <c r="E47" s="40"/>
+      <c r="F47" s="40">
         <f>F46-O22</f>
         <v>19</v>
       </c>
     </row>
     <row r="48" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E48" s="54"/>
-      <c r="F48" s="54">
+      <c r="E48" s="40"/>
+      <c r="F48" s="40">
         <f>F47-P22</f>
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E49" s="54">
+      <c r="E49" s="40">
         <v>0</v>
       </c>
-      <c r="F49" s="54">
-        <f ca="1">F48-Q22</f>
+      <c r="F49" s="40">
+        <f>F48-Q22</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="E39:F49"/>
   <mergeCells count="25">
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="D20:E20"/>
@@ -3929,14 +4978,20 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
U projektnu dokumentaciju dodane su slike SprintBackloga za drugi spirnt, BurnDown chart-a sa pripadajućim opisom. Također, dodan je opis održanih sastanaka te je dodan opis online alata Trello i način na koji smo ga koristili.
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
   <si>
     <t>Zadatak</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Dan 10</t>
+  </si>
+  <si>
+    <t>Početak 2.sprinta</t>
   </si>
 </sst>
 </file>
@@ -646,13 +649,16 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,22 +667,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,6 +686,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -745,7 +748,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -986,11 +988,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-852700128"/>
-        <c:axId val="-852127136"/>
+        <c:axId val="-1528086720"/>
+        <c:axId val="-1528092160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-852700128"/>
+        <c:axId val="-1528086720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,7 +1035,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-852127136"/>
+        <c:crossAx val="-1528092160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1041,7 +1043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-852127136"/>
+        <c:axId val="-1528092160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1094,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-852700128"/>
+        <c:crossAx val="-1528086720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1106,7 +1108,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1462,11 +1463,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-333479568"/>
-        <c:axId val="-333478480"/>
+        <c:axId val="-1528083456"/>
+        <c:axId val="-1528090528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-333479568"/>
+        <c:axId val="-1528083456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,7 +1510,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-333478480"/>
+        <c:crossAx val="-1528090528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1517,7 +1518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-333478480"/>
+        <c:axId val="-1528090528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1568,7 +1569,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-333479568"/>
+        <c:crossAx val="-1528083456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3083,27 +3084,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
@@ -3134,10 +3135,10 @@
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3174,10 +3175,10 @@
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="42"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="2">
         <v>4</v>
       </c>
@@ -3212,10 +3213,10 @@
     </row>
     <row r="5" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26"/>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="2">
         <v>2</v>
       </c>
@@ -3248,10 +3249,10 @@
       <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="42"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -3282,10 +3283,10 @@
     </row>
     <row r="7" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26"/>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="42"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -3308,10 +3309,10 @@
     </row>
     <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26"/>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -3336,10 +3337,10 @@
     </row>
     <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="44"/>
       <c r="E9" s="2">
         <v>4</v>
       </c>
@@ -3368,10 +3369,10 @@
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="42"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="2">
         <v>5</v>
       </c>
@@ -3408,10 +3409,10 @@
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="42"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="2">
         <v>2</v>
       </c>
@@ -3448,10 +3449,10 @@
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="42"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="2">
         <v>2</v>
       </c>
@@ -3488,10 +3489,10 @@
     </row>
     <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="42"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="2">
         <v>6</v>
       </c>
@@ -3526,10 +3527,10 @@
       <c r="B14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="42"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="12">
         <v>4</v>
       </c>
@@ -3556,10 +3557,10 @@
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29"/>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="45"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="12">
         <v>5</v>
       </c>
@@ -3598,10 +3599,10 @@
       <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="42"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="12">
         <v>4</v>
       </c>
@@ -3633,7 +3634,7 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="48"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -3642,7 +3643,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="48"/>
+      <c r="F17" s="41"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -3654,13 +3655,13 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="50"/>
+      <c r="F18" s="47"/>
       <c r="G18" s="8">
         <v>3</v>
       </c>
@@ -3690,7 +3691,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -3698,7 +3699,7 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="50"/>
+      <c r="F19" s="47"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
         <v>43</v>
@@ -3737,31 +3738,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="47" t="s">
+      <c r="G21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47" t="s">
+      <c r="H21" s="48"/>
+      <c r="I21" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="47"/>
+      <c r="J21" s="48"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
@@ -3771,14 +3772,14 @@
         <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47" t="s">
+      <c r="H22" s="48"/>
+      <c r="I22" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="47"/>
+      <c r="J22" s="48"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
@@ -3788,14 +3789,14 @@
         <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G23" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47">
+      <c r="H23" s="48"/>
+      <c r="I23" s="48">
         <v>9</v>
       </c>
-      <c r="J23" s="47"/>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -3831,116 +3832,92 @@
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="46"/>
+      <c r="H31" s="49"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="44">
+      <c r="G32" s="45">
         <f>F32-G18</f>
         <v>43</v>
       </c>
-      <c r="H32" s="45"/>
+      <c r="H32" s="46"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="44">
+      <c r="G33" s="45">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="45"/>
+      <c r="H33" s="46"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="44">
+      <c r="G34" s="45">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="45"/>
+      <c r="H34" s="46"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="44">
+      <c r="G35" s="45">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="45"/>
+      <c r="H35" s="46"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="44">
+      <c r="G36" s="45">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="45"/>
+      <c r="H36" s="46"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="44">
+      <c r="G37" s="45">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="45"/>
+      <c r="H37" s="46"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="44">
+      <c r="G38" s="45">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="45"/>
+      <c r="H38" s="46"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="44">
+      <c r="G39" s="45">
         <f>G38-N18</f>
         <v>8</v>
       </c>
-      <c r="H39" s="45"/>
+      <c r="H39" s="46"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="44">
+      <c r="G40" s="45">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="45"/>
+      <c r="H40" s="46"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="36">
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G20:O20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C12:D12"/>
@@ -3953,6 +3930,30 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3964,8 +3965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,28 +3987,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
       <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
       <c r="H4" s="31" t="s">
         <v>55</v>
       </c>
@@ -4041,10 +4042,10 @@
     </row>
     <row r="5" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="25"/>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="43"/>
+      <c r="E5" s="50"/>
       <c r="F5" s="21" t="s">
         <v>34</v>
       </c>
@@ -4084,10 +4085,10 @@
     </row>
     <row r="6" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C6" s="26"/>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="42"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="20">
         <v>9</v>
       </c>
@@ -4121,10 +4122,10 @@
     </row>
     <row r="7" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C7" s="26"/>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="44"/>
       <c r="F7" s="20">
         <v>5</v>
       </c>
@@ -4164,10 +4165,10 @@
       <c r="C8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="20">
         <v>2</v>
       </c>
@@ -4207,10 +4208,10 @@
       <c r="C9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="45"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="20">
         <v>4</v>
       </c>
@@ -4243,7 +4244,7 @@
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="51" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="23"/>
@@ -4286,7 +4287,7 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="53"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
         <v>64</v>
@@ -4323,11 +4324,11 @@
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="54"/>
-      <c r="D12" s="44" t="s">
+      <c r="C12" s="53"/>
+      <c r="D12" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="20">
         <v>2</v>
       </c>
@@ -4364,13 +4365,13 @@
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="45"/>
+      <c r="E13" s="46"/>
       <c r="F13" s="20">
         <v>4</v>
       </c>
@@ -4403,11 +4404,11 @@
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="53"/>
-      <c r="D14" s="44" t="s">
+      <c r="C14" s="52"/>
+      <c r="D14" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="45"/>
+      <c r="E14" s="46"/>
       <c r="F14" s="20">
         <v>6</v>
       </c>
@@ -4446,11 +4447,11 @@
       </c>
     </row>
     <row r="15" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="54"/>
-      <c r="D15" s="44" t="s">
+      <c r="C15" s="53"/>
+      <c r="D15" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="45"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="20">
         <v>2</v>
       </c>
@@ -4573,13 +4574,13 @@
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="42"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="20">
         <v>5</v>
       </c>
@@ -4610,11 +4611,11 @@
       <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="53"/>
-      <c r="D19" s="44" t="s">
+      <c r="C19" s="52"/>
+      <c r="D19" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="45"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="20">
         <v>8</v>
       </c>
@@ -4651,11 +4652,11 @@
       <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="54"/>
-      <c r="D20" s="42" t="s">
+      <c r="C20" s="53"/>
+      <c r="D20" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="42"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="20">
         <v>2</v>
       </c>
@@ -4692,7 +4693,7 @@
       <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="50"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
         <v>23</v>
@@ -4701,7 +4702,7 @@
         <f>SUM(F6:F20)</f>
         <v>62</v>
       </c>
-      <c r="G21" s="50"/>
+      <c r="G21" s="47"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -4714,13 +4715,13 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="41"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="50"/>
+      <c r="G22" s="47"/>
       <c r="H22" s="8">
         <v>0</v>
       </c>
@@ -4754,7 +4755,7 @@
       </c>
     </row>
     <row r="23" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="41"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>36</v>
@@ -4763,7 +4764,7 @@
         <f>F21</f>
         <v>62</v>
       </c>
-      <c r="G23" s="50"/>
+      <c r="G23" s="47"/>
       <c r="H23" s="8">
         <f>F23-H22</f>
         <v>62</v>
@@ -4809,14 +4810,14 @@
       <c r="F28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51" t="s">
+      <c r="I28" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="L28" s="51"/>
+      <c r="L28" s="54"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E29" s="3" t="s">
@@ -4826,14 +4827,14 @@
         <f>SUM(F18:F20)</f>
         <v>15</v>
       </c>
-      <c r="I29" s="51" t="s">
+      <c r="I29" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51" t="s">
+      <c r="J29" s="54"/>
+      <c r="K29" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="51"/>
+      <c r="L29" s="54"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E30" s="3" t="s">
@@ -4843,14 +4844,14 @@
         <f>SUM(F6:F8)</f>
         <v>16</v>
       </c>
-      <c r="I30" s="51" t="s">
+      <c r="I30" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51">
+      <c r="J30" s="54"/>
+      <c r="K30" s="54">
         <v>10</v>
       </c>
-      <c r="L30" s="51"/>
+      <c r="L30" s="54"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
@@ -4964,12 +4965,14 @@
   </sheetData>
   <autoFilter ref="E39:F49"/>
   <mergeCells count="25">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="D20:E20"/>
@@ -4981,14 +4984,12 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Kreiran je sprint backlog u Excelu te će se isti dalje nadopunjavati sa potrebnim podacima
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SprintBackLog 1" sheetId="1" r:id="rId1"/>
     <sheet name="SpirntBacklog 2" sheetId="2" r:id="rId2"/>
+    <sheet name="SprintBacklog 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SpirntBacklog 2'!$E$39:$F$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SprintBackLog 1'!$F$31:$H$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SprintBacklog 3'!$F$36:$G$43</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="110">
   <si>
     <t>Zadatak</t>
   </si>
@@ -281,6 +283,84 @@
   </si>
   <si>
     <t>Početak 2.sprinta</t>
+  </si>
+  <si>
+    <t>Mapni prikaz ljekarni</t>
+  </si>
+  <si>
+    <t>Dnevni raspored</t>
+  </si>
+  <si>
+    <t>Obavijesti</t>
+  </si>
+  <si>
+    <t>Kreirati aktivnost za mapni prikaz</t>
+  </si>
+  <si>
+    <t>Implementirati metode za prikaz ljekarni ovisno o korisnikovoj lokaciji</t>
+  </si>
+  <si>
+    <t>Kreirati aktivnost za dnevni raspored</t>
+  </si>
+  <si>
+    <t>Implementirati metode za prikaz dnevnog rasporeda</t>
+  </si>
+  <si>
+    <t>Implementirati metode za prikaz karte</t>
+  </si>
+  <si>
+    <t>Postaviti vremenski prikaz obavijesti</t>
+  </si>
+  <si>
+    <t>Kreirati potrebne aktivnosti za prikaz obavijesti</t>
+  </si>
+  <si>
+    <t>Implementirati metode za prikaz obavijesti o stanju tableta</t>
+  </si>
+  <si>
+    <t>Implementirati metode za prikaz obavijesti o nadolazećem pregledu</t>
+  </si>
+  <si>
+    <t>Implementirati metode za prikaz obavijesti o terapiji</t>
+  </si>
+  <si>
+    <t>Dokumentacija</t>
+  </si>
+  <si>
+    <t>Reorganiziranje tehničke dokumentacije</t>
+  </si>
+  <si>
+    <t>Izrada dijagrama</t>
+  </si>
+  <si>
+    <t>Izraditi dijagrama</t>
+  </si>
+  <si>
+    <t>09.01.2018.</t>
+  </si>
+  <si>
+    <t>11.01.2018.</t>
+  </si>
+  <si>
+    <t>13.01.2018.</t>
+  </si>
+  <si>
+    <t>22.01.2018.</t>
+  </si>
+  <si>
+    <t>20.01.2018.</t>
+  </si>
+  <si>
+    <t>15.01.2017.</t>
+  </si>
+  <si>
+    <t>18.01.2018.</t>
+  </si>
+  <si>
+    <t>Početak 3.sprinta</t>
+  </si>
+  <si>
+    <t>24.01.2018.</t>
   </si>
 </sst>
 </file>
@@ -539,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -649,31 +729,10 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -688,9 +747,50 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,11 +1088,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1528086720"/>
-        <c:axId val="-1528092160"/>
+        <c:axId val="-802958816"/>
+        <c:axId val="-802966976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1528086720"/>
+        <c:axId val="-802958816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,7 +1135,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1528092160"/>
+        <c:crossAx val="-802966976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1043,7 +1143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1528092160"/>
+        <c:axId val="-802966976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1094,7 +1194,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1528086720"/>
+        <c:crossAx val="-802958816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1463,11 +1563,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1528083456"/>
-        <c:axId val="-1528090528"/>
+        <c:axId val="-802955008"/>
+        <c:axId val="-802964800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1528083456"/>
+        <c:axId val="-802955008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,7 +1610,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1528090528"/>
+        <c:crossAx val="-802964800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1518,7 +1618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1528090528"/>
+        <c:axId val="-802964800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1569,7 +1669,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1528083456"/>
+        <c:crossAx val="-802955008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1614,6 +1714,443 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sr-Latn-RS"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hr-HR"/>
+              <a:t>BurnDown chart</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="hr-HR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sr-Latn-RS"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SprintBacklog 3'!$F$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Idealno</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SprintBacklog 3'!$I$5:$O$5</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>09.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.01.2017.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.01.2018.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SprintBacklog 3'!$F$37:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SprintBacklog 3'!$G$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Preostali napor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SprintBacklog 3'!$I$5:$O$5</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>09.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.01.2017.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.01.2018.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.01.2018.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SprintBacklog 3'!$G$37:$G$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-347890400"/>
+        <c:axId val="-347877888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-347890400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sr-Latn-RS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-347877888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-347877888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sr-Latn-RS"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-347890400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sr-Latn-RS"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="span"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
@@ -1730,6 +2267,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2731,6 +3308,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2788,6 +3881,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>386290</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>83608</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>232833</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3084,27 +4212,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
@@ -3135,10 +4263,10 @@
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3175,10 +4303,10 @@
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="2">
         <v>4</v>
       </c>
@@ -3213,10 +4341,10 @@
     </row>
     <row r="5" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26"/>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="2">
         <v>2</v>
       </c>
@@ -3249,10 +4377,10 @@
       <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="44"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -3283,10 +4411,10 @@
     </row>
     <row r="7" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26"/>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="44"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -3309,10 +4437,10 @@
     </row>
     <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26"/>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="44"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -3337,10 +4465,10 @@
     </row>
     <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="2">
         <v>4</v>
       </c>
@@ -3369,10 +4497,10 @@
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="2">
         <v>5</v>
       </c>
@@ -3409,10 +4537,10 @@
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="2">
         <v>2</v>
       </c>
@@ -3449,10 +4577,10 @@
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="44"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="2">
         <v>2</v>
       </c>
@@ -3489,10 +4617,10 @@
     </row>
     <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="44"/>
+      <c r="D13" s="48"/>
       <c r="E13" s="2">
         <v>6</v>
       </c>
@@ -3527,10 +4655,10 @@
       <c r="B14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="44"/>
+      <c r="D14" s="48"/>
       <c r="E14" s="12">
         <v>4</v>
       </c>
@@ -3557,10 +4685,10 @@
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29"/>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="46"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="12">
         <v>5</v>
       </c>
@@ -3599,10 +4727,10 @@
       <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="48"/>
       <c r="E16" s="12">
         <v>4</v>
       </c>
@@ -3634,7 +4762,7 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -3643,7 +4771,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="41"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -3655,13 +4783,13 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="47"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="8">
         <v>3</v>
       </c>
@@ -3691,7 +4819,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -3699,7 +4827,7 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="47"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
         <v>43</v>
@@ -3738,31 +4866,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48" t="s">
+      <c r="H21" s="53"/>
+      <c r="I21" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="48"/>
+      <c r="J21" s="53"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
@@ -3772,14 +4900,14 @@
         <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48" t="s">
+      <c r="H22" s="53"/>
+      <c r="I22" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="48"/>
+      <c r="J22" s="53"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
@@ -3789,14 +4917,14 @@
         <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="48" t="s">
+      <c r="G23" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48">
+      <c r="H23" s="53"/>
+      <c r="I23" s="53">
         <v>9</v>
       </c>
-      <c r="J23" s="48"/>
+      <c r="J23" s="53"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -3832,92 +4960,116 @@
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="49" t="s">
+      <c r="G31" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="49"/>
+      <c r="H31" s="52"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="45">
+      <c r="G32" s="50">
         <f>F32-G18</f>
         <v>43</v>
       </c>
-      <c r="H32" s="46"/>
+      <c r="H32" s="51"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="45">
+      <c r="G33" s="50">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="46"/>
+      <c r="H33" s="51"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="45">
+      <c r="G34" s="50">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="46"/>
+      <c r="H34" s="51"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="45">
+      <c r="G35" s="50">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="46"/>
+      <c r="H35" s="51"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="45">
+      <c r="G36" s="50">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="46"/>
+      <c r="H36" s="51"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="45">
+      <c r="G37" s="50">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="46"/>
+      <c r="H37" s="51"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="45">
+      <c r="G38" s="50">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="46"/>
+      <c r="H38" s="51"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="45">
+      <c r="G39" s="50">
         <f>G38-N18</f>
         <v>8</v>
       </c>
-      <c r="H39" s="46"/>
+      <c r="H39" s="51"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="45">
+      <c r="G40" s="50">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="46"/>
+      <c r="H40" s="51"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="36">
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G20:O20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C12:D12"/>
@@ -3930,30 +5082,6 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3965,8 +5093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView topLeftCell="E21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3987,28 +5115,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
       <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="31" t="s">
         <v>55</v>
       </c>
@@ -4042,10 +5170,10 @@
     </row>
     <row r="5" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="25"/>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="50"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="21" t="s">
         <v>34</v>
       </c>
@@ -4085,10 +5213,10 @@
     </row>
     <row r="6" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C6" s="26"/>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="20">
         <v>9</v>
       </c>
@@ -4122,10 +5250,10 @@
     </row>
     <row r="7" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C7" s="26"/>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="44"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="20">
         <v>5</v>
       </c>
@@ -4165,10 +5293,10 @@
       <c r="C8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="20">
         <v>2</v>
       </c>
@@ -4208,10 +5336,10 @@
       <c r="C9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="46"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="20">
         <v>4</v>
       </c>
@@ -4244,7 +5372,7 @@
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="58" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="23"/>
@@ -4287,7 +5415,7 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="52"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
         <v>64</v>
@@ -4324,11 +5452,11 @@
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="53"/>
-      <c r="D12" s="45" t="s">
+      <c r="C12" s="60"/>
+      <c r="D12" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="20">
         <v>2</v>
       </c>
@@ -4365,13 +5493,13 @@
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="51"/>
       <c r="F13" s="20">
         <v>4</v>
       </c>
@@ -4404,11 +5532,11 @@
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="52"/>
-      <c r="D14" s="45" t="s">
+      <c r="C14" s="59"/>
+      <c r="D14" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="46"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="20">
         <v>6</v>
       </c>
@@ -4447,11 +5575,11 @@
       </c>
     </row>
     <row r="15" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="53"/>
-      <c r="D15" s="45" t="s">
+      <c r="C15" s="60"/>
+      <c r="D15" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="46"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="20">
         <v>2</v>
       </c>
@@ -4574,13 +5702,13 @@
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="44"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="20">
         <v>5</v>
       </c>
@@ -4611,11 +5739,11 @@
       <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="52"/>
-      <c r="D19" s="45" t="s">
+      <c r="C19" s="59"/>
+      <c r="D19" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="46"/>
+      <c r="E19" s="51"/>
       <c r="F19" s="20">
         <v>8</v>
       </c>
@@ -4652,11 +5780,11 @@
       <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="53"/>
-      <c r="D20" s="44" t="s">
+      <c r="C20" s="60"/>
+      <c r="D20" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="44"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="20">
         <v>2</v>
       </c>
@@ -4693,7 +5821,7 @@
       <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="47"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
         <v>23</v>
@@ -4702,7 +5830,7 @@
         <f>SUM(F6:F20)</f>
         <v>62</v>
       </c>
-      <c r="G21" s="47"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -4715,13 +5843,13 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="42"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="47"/>
+      <c r="G22" s="56"/>
       <c r="H22" s="8">
         <v>0</v>
       </c>
@@ -4755,7 +5883,7 @@
       </c>
     </row>
     <row r="23" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="42"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>36</v>
@@ -4764,7 +5892,7 @@
         <f>F21</f>
         <v>62</v>
       </c>
-      <c r="G23" s="47"/>
+      <c r="G23" s="56"/>
       <c r="H23" s="8">
         <f>F23-H22</f>
         <v>62</v>
@@ -4810,14 +5938,14 @@
       <c r="F28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="54" t="s">
+      <c r="I28" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54" t="s">
+      <c r="J28" s="57"/>
+      <c r="K28" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="L28" s="54"/>
+      <c r="L28" s="57"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E29" s="3" t="s">
@@ -4827,14 +5955,14 @@
         <f>SUM(F18:F20)</f>
         <v>15</v>
       </c>
-      <c r="I29" s="54" t="s">
+      <c r="I29" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54" t="s">
+      <c r="J29" s="57"/>
+      <c r="K29" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="54"/>
+      <c r="L29" s="57"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E30" s="3" t="s">
@@ -4844,14 +5972,14 @@
         <f>SUM(F6:F8)</f>
         <v>16</v>
       </c>
-      <c r="I30" s="54" t="s">
+      <c r="I30" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54">
+      <c r="J30" s="57"/>
+      <c r="K30" s="57">
         <v>10</v>
       </c>
-      <c r="L30" s="54"/>
+      <c r="L30" s="57"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
@@ -4965,14 +6093,12 @@
   </sheetData>
   <autoFilter ref="E39:F49"/>
   <mergeCells count="25">
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="D20:E20"/>
@@ -4984,15 +6110,792 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:R43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="42"/>
+    </row>
+    <row r="5" spans="4:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+    </row>
+    <row r="6" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D6" s="44"/>
+      <c r="E6" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D7" s="45"/>
+      <c r="E7" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="48"/>
+      <c r="G7" s="41">
+        <v>1</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="41">
+        <v>9</v>
+      </c>
+      <c r="J7" s="41">
+        <v>9</v>
+      </c>
+      <c r="K7" s="41">
+        <v>9</v>
+      </c>
+      <c r="L7" s="13">
+        <v>9</v>
+      </c>
+      <c r="M7" s="41">
+        <v>9</v>
+      </c>
+      <c r="N7" s="41">
+        <v>4</v>
+      </c>
+      <c r="O7" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D8" s="45"/>
+      <c r="E8" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="48"/>
+      <c r="G8" s="41">
+        <v>2</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="41">
+        <v>5</v>
+      </c>
+      <c r="J8" s="41">
+        <v>5</v>
+      </c>
+      <c r="K8" s="41">
+        <v>5</v>
+      </c>
+      <c r="L8" s="41">
+        <v>5</v>
+      </c>
+      <c r="M8" s="41">
+        <v>3</v>
+      </c>
+      <c r="N8" s="35">
+        <v>1</v>
+      </c>
+      <c r="O8" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D9" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="48"/>
+      <c r="G9" s="41">
+        <v>2</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="41">
+        <v>2</v>
+      </c>
+      <c r="J9" s="41">
+        <v>2</v>
+      </c>
+      <c r="K9" s="41">
+        <v>2</v>
+      </c>
+      <c r="L9" s="41">
+        <v>2</v>
+      </c>
+      <c r="M9" s="41">
+        <v>2</v>
+      </c>
+      <c r="N9" s="35">
+        <v>2</v>
+      </c>
+      <c r="O9" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D10" s="46"/>
+      <c r="E10" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="51"/>
+      <c r="G10" s="41">
+        <v>2</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="41"/>
+    </row>
+    <row r="11" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="51"/>
+      <c r="G11" s="41">
+        <v>3</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="41"/>
+    </row>
+    <row r="12" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="60"/>
+      <c r="E12" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="41">
+        <v>2</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="41"/>
+    </row>
+    <row r="13" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="51"/>
+      <c r="G13" s="41">
+        <v>2</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="41">
+        <v>4</v>
+      </c>
+      <c r="J13" s="41">
+        <v>4</v>
+      </c>
+      <c r="K13" s="41">
+        <v>4</v>
+      </c>
+      <c r="L13" s="35">
+        <v>4</v>
+      </c>
+      <c r="M13" s="41">
+        <v>4</v>
+      </c>
+      <c r="N13" s="41">
+        <v>3</v>
+      </c>
+      <c r="O13" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="59"/>
+      <c r="E14" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="41">
+        <v>5</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="60"/>
+      <c r="E15" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="51"/>
+      <c r="G15" s="41">
+        <v>2</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="36"/>
+    </row>
+    <row r="16" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D16" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="51"/>
+      <c r="G16" s="41">
+        <v>2</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="41">
+        <v>4</v>
+      </c>
+      <c r="J16" s="41">
+        <v>4</v>
+      </c>
+      <c r="K16" s="41">
+        <v>4</v>
+      </c>
+      <c r="L16" s="41">
+        <v>4</v>
+      </c>
+      <c r="M16" s="41">
+        <v>4</v>
+      </c>
+      <c r="N16" s="41">
+        <v>4</v>
+      </c>
+      <c r="O16" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D17" s="59"/>
+      <c r="E17" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="41">
+        <v>3</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="41">
+        <v>2</v>
+      </c>
+      <c r="J17" s="41">
+        <v>2</v>
+      </c>
+      <c r="K17" s="41">
+        <v>2</v>
+      </c>
+      <c r="L17" s="41">
+        <v>2</v>
+      </c>
+      <c r="M17" s="41">
+        <v>2</v>
+      </c>
+      <c r="N17" s="41">
+        <v>2</v>
+      </c>
+      <c r="O17" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D18" s="59"/>
+      <c r="E18" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="41">
+        <v>2</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="36"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D19" s="59"/>
+      <c r="E19" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="41">
+        <v>3</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="36"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="59"/>
+      <c r="E20" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="41">
+        <v>3</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="36"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D21" s="60"/>
+      <c r="E21" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="41">
+        <v>3</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="41">
+        <v>2</v>
+      </c>
+      <c r="J21" s="41">
+        <v>2</v>
+      </c>
+      <c r="K21" s="41">
+        <v>2</v>
+      </c>
+      <c r="L21" s="41">
+        <v>2</v>
+      </c>
+      <c r="M21" s="41">
+        <v>2</v>
+      </c>
+      <c r="N21" s="41">
+        <v>2</v>
+      </c>
+      <c r="O21" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D22" s="56"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="8">
+        <f>SUM(G7:G21)</f>
+        <v>37</v>
+      </c>
+      <c r="H22" s="56"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="47"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="8">
+        <v>2</v>
+      </c>
+      <c r="J23" s="8">
+        <v>3</v>
+      </c>
+      <c r="K23" s="8">
+        <v>4</v>
+      </c>
+      <c r="L23" s="8">
+        <v>5</v>
+      </c>
+      <c r="M23" s="8">
+        <v>4</v>
+      </c>
+      <c r="N23" s="8">
+        <v>3</v>
+      </c>
+      <c r="O23" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D24" s="47"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="8">
+        <f>G22</f>
+        <v>37</v>
+      </c>
+      <c r="H24" s="56"/>
+      <c r="I24" s="8">
+        <f>G24-I23</f>
+        <v>35</v>
+      </c>
+      <c r="J24" s="8">
+        <f>I24-J23</f>
+        <v>32</v>
+      </c>
+      <c r="K24" s="8">
+        <f t="shared" ref="K24:L24" si="0">J24-K23</f>
+        <v>28</v>
+      </c>
+      <c r="L24" s="8">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="M24" s="8">
+        <f>L24-M23</f>
+        <v>19</v>
+      </c>
+      <c r="N24" s="8">
+        <f>M24-N23</f>
+        <v>16</v>
+      </c>
+      <c r="O24" s="8">
+        <f>N24-O23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F29" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29" s="57"/>
+      <c r="M29" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F30" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30" s="57"/>
+      <c r="L30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="4">
+        <f>SUM(G11:G12)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F31" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57">
+        <v>7</v>
+      </c>
+      <c r="I31" s="57"/>
+      <c r="L31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="4">
+        <f>SUM(G7:G10)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" s="4">
+        <f>SUM(G16:G21)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33" s="4">
+        <f>SUM(G13:G15)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L34" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" s="9">
+        <f>SUM(M30:M33)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F36" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F37" s="40">
+        <f>G22</f>
+        <v>37</v>
+      </c>
+      <c r="G37" s="40">
+        <f>F37-I23</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F38" s="40"/>
+      <c r="G38" s="40">
+        <f>G37-J23</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F39" s="40"/>
+      <c r="G39" s="40">
+        <f>J24-K23</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F40" s="40"/>
+      <c r="G40" s="40">
+        <f>K24-L23</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F41" s="40"/>
+      <c r="G41" s="40">
+        <f>G40-M23</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F42" s="40"/>
+      <c r="G42" s="40">
+        <f>G41-N23</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F43" s="40">
+        <v>0</v>
+      </c>
+      <c r="G43" s="40">
+        <f>G42-O23</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="F36:G43"/>
+  <mergeCells count="28">
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="D16:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="D4:H5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Nadopunjen je i popravljen SprintBacklog
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SpirntBacklog 2'!$E$39:$F$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SprintBackLog 1'!$F$31:$H$40</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SprintBacklog 3'!$F$36:$G$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SprintBacklog 3'!$F$34:$G$41</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="107">
   <si>
     <t>Zadatak</t>
   </si>
@@ -324,18 +324,6 @@
     <t>Implementirati metode za prikaz obavijesti o terapiji</t>
   </si>
   <si>
-    <t>Dokumentacija</t>
-  </si>
-  <si>
-    <t>Reorganiziranje tehničke dokumentacije</t>
-  </si>
-  <si>
-    <t>Izrada dijagrama</t>
-  </si>
-  <si>
-    <t>Izraditi dijagrama</t>
-  </si>
-  <si>
     <t>09.01.2018.</t>
   </si>
   <si>
@@ -361,6 +349,9 @@
   </si>
   <si>
     <t>24.01.2018.</t>
+  </si>
+  <si>
+    <t>Izraditi dijagrame</t>
   </si>
 </sst>
 </file>
@@ -747,13 +738,18 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -762,22 +758,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,8 +779,9 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,11 +1079,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-802958816"/>
-        <c:axId val="-802966976"/>
+        <c:axId val="1839971824"/>
+        <c:axId val="1839983792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-802958816"/>
+        <c:axId val="1839971824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1126,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-802966976"/>
+        <c:crossAx val="1839983792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1143,7 +1134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-802966976"/>
+        <c:axId val="1839983792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,7 +1185,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-802958816"/>
+        <c:crossAx val="1839971824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1313,7 +1304,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1563,11 +1553,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-802955008"/>
-        <c:axId val="-802964800"/>
+        <c:axId val="1839979440"/>
+        <c:axId val="1839972368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-802955008"/>
+        <c:axId val="1839979440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1600,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-802964800"/>
+        <c:crossAx val="1839972368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1618,7 +1608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-802964800"/>
+        <c:axId val="1839972368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1659,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-802955008"/>
+        <c:crossAx val="1839979440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1683,7 +1673,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1837,7 +1826,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SprintBacklog 3'!$F$36</c:f>
+              <c:f>'SprintBacklog 3'!$F$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1889,12 +1878,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SprintBacklog 3'!$F$37:$F$43</c:f>
+              <c:f>'SprintBacklog 3'!$F$35:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1909,7 +1898,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SprintBacklog 3'!$G$36</c:f>
+              <c:f>'SprintBacklog 3'!$G$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1961,30 +1950,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SprintBacklog 3'!$G$37:$G$43</c:f>
+              <c:f>'SprintBacklog 3'!$G$35:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2000,11 +1989,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-347890400"/>
-        <c:axId val="-347877888"/>
+        <c:axId val="1838604944"/>
+        <c:axId val="1838605488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-347890400"/>
+        <c:axId val="1838604944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2047,7 +2036,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-347877888"/>
+        <c:crossAx val="1838605488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2055,7 +2044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-347877888"/>
+        <c:axId val="1838605488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2106,7 +2095,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-347890400"/>
+        <c:crossAx val="1838604944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3904,13 +3893,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>386290</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>83608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>232833</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4212,27 +4201,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
@@ -4263,10 +4252,10 @@
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -4303,10 +4292,10 @@
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2">
         <v>4</v>
       </c>
@@ -4341,10 +4330,10 @@
     </row>
     <row r="5" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26"/>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="2">
         <v>2</v>
       </c>
@@ -4377,10 +4366,10 @@
       <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -4411,10 +4400,10 @@
     </row>
     <row r="7" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26"/>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -4437,10 +4426,10 @@
     </row>
     <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26"/>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="52"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -4465,10 +4454,10 @@
     </row>
     <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="2">
         <v>4</v>
       </c>
@@ -4497,10 +4486,10 @@
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="2">
         <v>5</v>
       </c>
@@ -4537,10 +4526,10 @@
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="2">
         <v>2</v>
       </c>
@@ -4577,10 +4566,10 @@
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="52"/>
       <c r="E12" s="2">
         <v>2</v>
       </c>
@@ -4617,10 +4606,10 @@
     </row>
     <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="48"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="2">
         <v>6</v>
       </c>
@@ -4655,10 +4644,10 @@
       <c r="B14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="12">
         <v>4</v>
       </c>
@@ -4685,10 +4674,10 @@
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29"/>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="54"/>
       <c r="E15" s="12">
         <v>5</v>
       </c>
@@ -4727,10 +4716,10 @@
       <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="12">
         <v>4</v>
       </c>
@@ -4762,7 +4751,7 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="54"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -4771,7 +4760,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="54"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -4783,13 +4772,13 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="56"/>
+      <c r="F18" s="55"/>
       <c r="G18" s="8">
         <v>3</v>
       </c>
@@ -4819,7 +4808,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -4827,7 +4816,7 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="56"/>
+      <c r="F19" s="55"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
         <v>43</v>
@@ -4866,31 +4855,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="53" t="s">
+      <c r="G21" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53" t="s">
+      <c r="H21" s="56"/>
+      <c r="I21" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="53"/>
+      <c r="J21" s="56"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
@@ -4900,14 +4889,14 @@
         <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53" t="s">
+      <c r="H22" s="56"/>
+      <c r="I22" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="53"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
@@ -4917,14 +4906,14 @@
         <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="53" t="s">
+      <c r="G23" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53">
+      <c r="H23" s="56"/>
+      <c r="I23" s="56">
         <v>9</v>
       </c>
-      <c r="J23" s="53"/>
+      <c r="J23" s="56"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -4960,116 +4949,92 @@
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="52" t="s">
+      <c r="G31" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="52"/>
+      <c r="H31" s="57"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="50">
+      <c r="G32" s="53">
         <f>F32-G18</f>
         <v>43</v>
       </c>
-      <c r="H32" s="51"/>
+      <c r="H32" s="54"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="50">
+      <c r="G33" s="53">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="51"/>
+      <c r="H33" s="54"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="50">
+      <c r="G34" s="53">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="51"/>
+      <c r="H34" s="54"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="50">
+      <c r="G35" s="53">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="51"/>
+      <c r="H35" s="54"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="50">
+      <c r="G36" s="53">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="51"/>
+      <c r="H36" s="54"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="50">
+      <c r="G37" s="53">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="51"/>
+      <c r="H37" s="54"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="50">
+      <c r="G38" s="53">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="51"/>
+      <c r="H38" s="54"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="50">
+      <c r="G39" s="53">
         <f>G38-N18</f>
         <v>8</v>
       </c>
-      <c r="H39" s="51"/>
+      <c r="H39" s="54"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="50">
+      <c r="G40" s="53">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="51"/>
+      <c r="H40" s="54"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="36">
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G20:O20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C12:D12"/>
@@ -5082,6 +5047,30 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -5115,28 +5104,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
       <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="31" t="s">
         <v>55</v>
       </c>
@@ -5170,10 +5159,10 @@
     </row>
     <row r="5" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="25"/>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="58"/>
       <c r="F5" s="21" t="s">
         <v>34</v>
       </c>
@@ -5213,10 +5202,10 @@
     </row>
     <row r="6" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C6" s="26"/>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="48"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="20">
         <v>9</v>
       </c>
@@ -5250,10 +5239,10 @@
     </row>
     <row r="7" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C7" s="26"/>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="48"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="20">
         <v>5</v>
       </c>
@@ -5293,10 +5282,10 @@
       <c r="C8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="48"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="20">
         <v>2</v>
       </c>
@@ -5336,10 +5325,10 @@
       <c r="C9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="51"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="20">
         <v>4</v>
       </c>
@@ -5372,7 +5361,7 @@
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="59" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="23"/>
@@ -5415,7 +5404,7 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="59"/>
+      <c r="C11" s="60"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
         <v>64</v>
@@ -5452,11 +5441,11 @@
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="60"/>
-      <c r="D12" s="50" t="s">
+      <c r="C12" s="61"/>
+      <c r="D12" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="20">
         <v>2</v>
       </c>
@@ -5493,13 +5482,13 @@
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="51"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="20">
         <v>4</v>
       </c>
@@ -5532,11 +5521,11 @@
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="59"/>
-      <c r="D14" s="50" t="s">
+      <c r="C14" s="60"/>
+      <c r="D14" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="51"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="20">
         <v>6</v>
       </c>
@@ -5575,11 +5564,11 @@
       </c>
     </row>
     <row r="15" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="60"/>
-      <c r="D15" s="50" t="s">
+      <c r="C15" s="61"/>
+      <c r="D15" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="51"/>
+      <c r="E15" s="54"/>
       <c r="F15" s="20">
         <v>2</v>
       </c>
@@ -5702,13 +5691,13 @@
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="48"/>
+      <c r="E18" s="52"/>
       <c r="F18" s="20">
         <v>5</v>
       </c>
@@ -5739,11 +5728,11 @@
       <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="59"/>
-      <c r="D19" s="50" t="s">
+      <c r="C19" s="60"/>
+      <c r="D19" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="51"/>
+      <c r="E19" s="54"/>
       <c r="F19" s="20">
         <v>8</v>
       </c>
@@ -5780,11 +5769,11 @@
       <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="60"/>
-      <c r="D20" s="48" t="s">
+      <c r="C20" s="61"/>
+      <c r="D20" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="48"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="20">
         <v>2</v>
       </c>
@@ -5821,7 +5810,7 @@
       <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="56"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
         <v>23</v>
@@ -5830,7 +5819,7 @@
         <f>SUM(F6:F20)</f>
         <v>62</v>
       </c>
-      <c r="G21" s="56"/>
+      <c r="G21" s="55"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -5843,13 +5832,13 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="47"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="56"/>
+      <c r="G22" s="55"/>
       <c r="H22" s="8">
         <v>0</v>
       </c>
@@ -5883,7 +5872,7 @@
       </c>
     </row>
     <row r="23" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="47"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>36</v>
@@ -5892,7 +5881,7 @@
         <f>F21</f>
         <v>62</v>
       </c>
-      <c r="G23" s="56"/>
+      <c r="G23" s="55"/>
       <c r="H23" s="8">
         <f>F23-H22</f>
         <v>62</v>
@@ -5938,14 +5927,14 @@
       <c r="F28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="57" t="s">
+      <c r="I28" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57" t="s">
+      <c r="J28" s="62"/>
+      <c r="K28" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="L28" s="57"/>
+      <c r="L28" s="62"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E29" s="3" t="s">
@@ -5955,14 +5944,14 @@
         <f>SUM(F18:F20)</f>
         <v>15</v>
       </c>
-      <c r="I29" s="57" t="s">
+      <c r="I29" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57" t="s">
+      <c r="J29" s="62"/>
+      <c r="K29" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="57"/>
+      <c r="L29" s="62"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E30" s="3" t="s">
@@ -5972,14 +5961,14 @@
         <f>SUM(F6:F8)</f>
         <v>16</v>
       </c>
-      <c r="I30" s="57" t="s">
+      <c r="I30" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57">
+      <c r="J30" s="62"/>
+      <c r="K30" s="62">
         <v>10</v>
       </c>
-      <c r="L30" s="57"/>
+      <c r="L30" s="62"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
@@ -6093,12 +6082,14 @@
   </sheetData>
   <autoFilter ref="E39:F49"/>
   <mergeCells count="25">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="D20:E20"/>
@@ -6110,14 +6101,12 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6127,10 +6116,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:R43"/>
+  <dimension ref="C4:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6152,58 +6141,58 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
       <c r="R4" s="42"/>
     </row>
     <row r="5" spans="4:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>105</v>
-      </c>
       <c r="O5" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
+        <v>100</v>
+      </c>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
     </row>
     <row r="6" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D6" s="44"/>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="49"/>
+      <c r="F6" s="58"/>
       <c r="G6" s="43" t="s">
         <v>34</v>
       </c>
@@ -6234,10 +6223,10 @@
     </row>
     <row r="7" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D7" s="45"/>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="48"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="41">
         <v>1</v>
       </c>
@@ -6268,10 +6257,10 @@
     </row>
     <row r="8" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D8" s="45"/>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="48"/>
+      <c r="F8" s="52"/>
       <c r="G8" s="41">
         <v>2</v>
       </c>
@@ -6304,12 +6293,12 @@
       <c r="D9" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="48"/>
+      <c r="F9" s="52"/>
       <c r="G9" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9" s="41" t="s">
         <v>25</v>
@@ -6338,15 +6327,15 @@
     </row>
     <row r="10" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D10" s="46"/>
-      <c r="E10" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="51"/>
+      <c r="E10" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="54"/>
       <c r="G10" s="41">
         <v>2</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
@@ -6358,200 +6347,198 @@
     </row>
     <row r="11" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="59" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="51"/>
+        <v>85</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="54"/>
       <c r="G11" s="41">
+        <v>2</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="41">
+        <v>4</v>
+      </c>
+      <c r="J11" s="41">
+        <v>4</v>
+      </c>
+      <c r="K11" s="41">
+        <v>4</v>
+      </c>
+      <c r="L11" s="35">
+        <v>4</v>
+      </c>
+      <c r="M11" s="41">
+        <v>4</v>
+      </c>
+      <c r="N11" s="41">
         <v>3</v>
       </c>
-      <c r="H11" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="41"/>
+      <c r="O11" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="60"/>
-      <c r="E12" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="51"/>
+      <c r="E12" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="54"/>
       <c r="G12" s="41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I12" s="41"/>
       <c r="J12" s="41"/>
       <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
+      <c r="L12" s="35"/>
       <c r="M12" s="41"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="36"/>
     </row>
     <row r="13" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="51"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="54"/>
       <c r="G13" s="41">
         <v>2</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="41">
+        <v>24</v>
+      </c>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="36"/>
+    </row>
+    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D14" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="54"/>
+      <c r="G14" s="41">
+        <v>2</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="41">
         <v>4</v>
       </c>
-      <c r="J13" s="41">
+      <c r="J14" s="41">
         <v>4</v>
       </c>
-      <c r="K13" s="41">
+      <c r="K14" s="41">
         <v>4</v>
       </c>
-      <c r="L13" s="35">
+      <c r="L14" s="41">
         <v>4</v>
       </c>
-      <c r="M13" s="41">
+      <c r="M14" s="41">
         <v>4</v>
       </c>
-      <c r="N13" s="41">
+      <c r="N14" s="41">
+        <v>4</v>
+      </c>
+      <c r="O14" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D15" s="60"/>
+      <c r="E15" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="54"/>
+      <c r="G15" s="41">
         <v>3</v>
       </c>
-      <c r="O13" s="36">
+      <c r="H15" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="41">
+        <v>2</v>
+      </c>
+      <c r="J15" s="41">
+        <v>2</v>
+      </c>
+      <c r="K15" s="41">
+        <v>2</v>
+      </c>
+      <c r="L15" s="41">
+        <v>2</v>
+      </c>
+      <c r="M15" s="41">
+        <v>2</v>
+      </c>
+      <c r="N15" s="41">
+        <v>2</v>
+      </c>
+      <c r="O15" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="59"/>
-      <c r="E14" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="41">
-        <v>5</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="36"/>
-    </row>
-    <row r="15" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="60"/>
-      <c r="E15" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="51"/>
-      <c r="G15" s="41">
-        <v>2</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="36"/>
-    </row>
     <row r="16" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D16" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="51"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="54"/>
       <c r="G16" s="41">
         <v>2</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="41">
-        <v>4</v>
-      </c>
-      <c r="J16" s="41">
-        <v>4</v>
-      </c>
-      <c r="K16" s="41">
-        <v>4</v>
-      </c>
-      <c r="L16" s="41">
-        <v>4</v>
-      </c>
-      <c r="M16" s="41">
-        <v>4</v>
-      </c>
-      <c r="N16" s="41">
-        <v>4</v>
-      </c>
-      <c r="O16" s="41">
-        <v>2</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="36"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="59"/>
-      <c r="E17" s="50" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="51"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="54"/>
       <c r="G17" s="41">
         <v>3</v>
       </c>
       <c r="H17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="41">
-        <v>2</v>
-      </c>
-      <c r="J17" s="41">
-        <v>2</v>
-      </c>
-      <c r="K17" s="41">
-        <v>2</v>
-      </c>
-      <c r="L17" s="41">
-        <v>2</v>
-      </c>
-      <c r="M17" s="41">
-        <v>2</v>
-      </c>
-      <c r="N17" s="41">
-        <v>2</v>
-      </c>
-      <c r="O17" s="36">
-        <v>0</v>
-      </c>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="36"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="59"/>
-      <c r="E18" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="51"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="54"/>
       <c r="G18" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="41" t="s">
         <v>27</v>
@@ -6565,335 +6552,292 @@
       <c r="O18" s="36"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="59"/>
-      <c r="E19" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="51"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="54"/>
       <c r="G19" s="41">
         <v>3</v>
       </c>
       <c r="H19" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="36"/>
-    </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="59"/>
-      <c r="E20" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="41">
+      <c r="I19" s="41">
+        <v>2</v>
+      </c>
+      <c r="J19" s="41">
+        <v>2</v>
+      </c>
+      <c r="K19" s="41">
+        <v>2</v>
+      </c>
+      <c r="L19" s="41">
+        <v>2</v>
+      </c>
+      <c r="M19" s="41">
+        <v>2</v>
+      </c>
+      <c r="N19" s="41">
+        <v>2</v>
+      </c>
+      <c r="O19" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D20" s="55"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="8">
+        <f>SUM(G7:G19)</f>
+        <v>34</v>
+      </c>
+      <c r="H20" s="55"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D21" s="50"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="8">
+        <v>2</v>
+      </c>
+      <c r="J21" s="8">
         <v>3</v>
       </c>
-      <c r="H20" s="41" t="s">
+      <c r="K21" s="8">
+        <v>4</v>
+      </c>
+      <c r="L21" s="8">
+        <v>5</v>
+      </c>
+      <c r="M21" s="8">
+        <v>4</v>
+      </c>
+      <c r="N21" s="8">
+        <v>3</v>
+      </c>
+      <c r="O21" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D22" s="50"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="8">
+        <f>G20</f>
+        <v>34</v>
+      </c>
+      <c r="H22" s="55"/>
+      <c r="I22" s="8">
+        <f>G22-I21</f>
+        <v>32</v>
+      </c>
+      <c r="J22" s="8">
+        <f>I22-J21</f>
+        <v>29</v>
+      </c>
+      <c r="K22" s="8">
+        <f t="shared" ref="K22:L22" si="0">J22-K21</f>
+        <v>25</v>
+      </c>
+      <c r="L22" s="8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M22" s="8">
+        <f>L22-M21</f>
+        <v>16</v>
+      </c>
+      <c r="N22" s="8">
+        <f>M22-N21</f>
+        <v>13</v>
+      </c>
+      <c r="O22" s="8">
+        <f>N22-O21</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F27" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="I27" s="62"/>
+      <c r="M27" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F28" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="I28" s="62"/>
+      <c r="L28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="4">
+        <f>SUM(G10,G13,G16)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F29" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62">
+        <v>7</v>
+      </c>
+      <c r="I29" s="62"/>
+      <c r="L29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="4">
+        <f>SUM(G7:G9)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="36"/>
-    </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D21" s="60"/>
-      <c r="E21" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="51"/>
-      <c r="G21" s="41">
-        <v>3</v>
-      </c>
-      <c r="H21" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="41">
-        <v>2</v>
-      </c>
-      <c r="J21" s="41">
-        <v>2</v>
-      </c>
-      <c r="K21" s="41">
-        <v>2</v>
-      </c>
-      <c r="L21" s="41">
-        <v>2</v>
-      </c>
-      <c r="M21" s="41">
-        <v>2</v>
-      </c>
-      <c r="N21" s="41">
-        <v>2</v>
-      </c>
-      <c r="O21" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D22" s="56"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="5" t="s">
+      <c r="M30" s="4">
+        <f>SUM(G14:G15,G17:G19)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31" s="4">
+        <f>SUM(G11:G12)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="8">
-        <f>SUM(G7:G21)</f>
+      <c r="M32" s="9">
+        <f>SUM(M28:M31)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F34" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D23" s="47"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="8">
-        <v>2</v>
-      </c>
-      <c r="J23" s="8">
-        <v>3</v>
-      </c>
-      <c r="K23" s="8">
-        <v>4</v>
-      </c>
-      <c r="L23" s="8">
-        <v>5</v>
-      </c>
-      <c r="M23" s="8">
-        <v>4</v>
-      </c>
-      <c r="N23" s="8">
-        <v>3</v>
-      </c>
-      <c r="O23" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D24" s="47"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="8">
-        <f>G22</f>
-        <v>37</v>
-      </c>
-      <c r="H24" s="56"/>
-      <c r="I24" s="8">
-        <f>G24-I23</f>
-        <v>35</v>
-      </c>
-      <c r="J24" s="8">
-        <f>I24-J23</f>
+      <c r="G34" s="39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F35" s="40">
+        <f>G20</f>
+        <v>34</v>
+      </c>
+      <c r="G35" s="40">
+        <f>F35-I21</f>
         <v>32</v>
       </c>
-      <c r="K24" s="8">
-        <f t="shared" ref="K24:L24" si="0">J24-K23</f>
-        <v>28</v>
-      </c>
-      <c r="L24" s="8">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="M24" s="8">
-        <f>L24-M23</f>
-        <v>19</v>
-      </c>
-      <c r="N24" s="8">
-        <f>M24-N23</f>
-        <v>16</v>
-      </c>
-      <c r="O24" s="8">
-        <f>N24-O23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F29" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="57"/>
-      <c r="M29" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F30" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="I30" s="57"/>
-      <c r="L30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M30" s="4">
-        <f>SUM(G11:G12)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F31" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57">
-        <v>7</v>
-      </c>
-      <c r="I31" s="57"/>
-      <c r="L31" s="3" t="s">
+    </row>
+    <row r="36" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F36" s="40"/>
+      <c r="G36" s="40">
+        <f>G35-J21</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F37" s="40"/>
+      <c r="G37" s="40">
+        <f>J22-K21</f>
         <v>25</v>
       </c>
-      <c r="M31" s="4">
-        <f>SUM(G7:G10)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="L32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M32" s="4">
-        <f>SUM(G16:G21)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M33" s="4">
-        <f>SUM(G13:G15)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L34" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M34" s="9">
-        <f>SUM(M30:M33)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F36" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G36" s="39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F37" s="40">
-        <f>G22</f>
-        <v>37</v>
-      </c>
-      <c r="G37" s="40">
-        <f>F37-I23</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F38" s="40"/>
       <c r="G38" s="40">
-        <f>G37-J23</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+        <f>K22-L21</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F39" s="40"/>
       <c r="G39" s="40">
-        <f>J24-K23</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+        <f>G38-M21</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F40" s="40"/>
       <c r="G40" s="40">
-        <f>K24-L23</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F41" s="40"/>
+        <f>G39-N21</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F41" s="40">
+        <v>0</v>
+      </c>
       <c r="G41" s="40">
-        <f>G40-M23</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F42" s="40"/>
-      <c r="G42" s="40">
-        <f>G41-N23</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F43" s="40">
-        <v>0</v>
-      </c>
-      <c r="G43" s="40">
-        <f>G42-O23</f>
-        <v>0</v>
+        <f>G40-O21</f>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F36:G43"/>
-  <mergeCells count="28">
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="D16:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E19:F19"/>
+  <autoFilter ref="F34:G41"/>
+  <mergeCells count="25">
     <mergeCell ref="D4:H5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Nadopunjen je SprintBacklog sa novim zadacima
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SpirntBacklog 2'!$E$39:$F$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SprintBackLog 1'!$F$31:$H$40</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SprintBacklog 3'!$F$34:$G$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SprintBacklog 3'!$F$37:$G$44</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="111">
   <si>
     <t>Zadatak</t>
   </si>
@@ -352,6 +352,18 @@
   </si>
   <si>
     <t>Izraditi dijagrame</t>
+  </si>
+  <si>
+    <t>Testiranje</t>
+  </si>
+  <si>
+    <t>Pripremiti okolinu za rad i testiranje</t>
+  </si>
+  <si>
+    <t>Pokrenuti testiranja</t>
+  </si>
+  <si>
+    <t>Analizirati i usporediti rezultate</t>
   </si>
 </sst>
 </file>
@@ -610,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -740,16 +752,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -758,16 +773,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -777,9 +798,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1079,11 +1097,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1839971824"/>
-        <c:axId val="1839983792"/>
+        <c:axId val="1718956016"/>
+        <c:axId val="1718956560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1839971824"/>
+        <c:axId val="1718956016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,7 +1144,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839983792"/>
+        <c:crossAx val="1718956560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1134,7 +1152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1839983792"/>
+        <c:axId val="1718956560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1203,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839971824"/>
+        <c:crossAx val="1718956016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1553,11 +1571,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1839979440"/>
-        <c:axId val="1839972368"/>
+        <c:axId val="1718959280"/>
+        <c:axId val="1718962000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1839979440"/>
+        <c:axId val="1718959280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1600,7 +1618,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839972368"/>
+        <c:crossAx val="1718962000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1608,7 +1626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1839972368"/>
+        <c:axId val="1718962000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,7 +1677,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839979440"/>
+        <c:crossAx val="1718959280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1826,7 +1844,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SprintBacklog 3'!$F$34</c:f>
+              <c:f>'SprintBacklog 3'!$F$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1878,12 +1896,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SprintBacklog 3'!$F$35:$F$41</c:f>
+              <c:f>'SprintBacklog 3'!$F$38:$F$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1898,7 +1916,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SprintBacklog 3'!$G$34</c:f>
+              <c:f>'SprintBacklog 3'!$G$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1950,30 +1968,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SprintBacklog 3'!$G$35:$G$41</c:f>
+              <c:f>'SprintBacklog 3'!$G$38:$G$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1989,11 +2007,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1838604944"/>
-        <c:axId val="1838605488"/>
+        <c:axId val="1722025152"/>
+        <c:axId val="1722033312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1838604944"/>
+        <c:axId val="1722025152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,7 +2054,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1838605488"/>
+        <c:crossAx val="1722033312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2044,7 +2062,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1838605488"/>
+        <c:axId val="1722033312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,7 +2113,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1838604944"/>
+        <c:crossAx val="1722025152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3893,13 +3911,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>386290</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>83608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>232833</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4201,27 +4219,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
@@ -4252,10 +4270,10 @@
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -4674,10 +4692,10 @@
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29"/>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="54"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="12">
         <v>5</v>
       </c>
@@ -4751,7 +4769,7 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="49"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -4760,7 +4778,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="49"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -4772,13 +4790,13 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="50"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="55"/>
+      <c r="F18" s="60"/>
       <c r="G18" s="8">
         <v>3</v>
       </c>
@@ -4808,7 +4826,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="50"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -4816,7 +4834,7 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="55"/>
+      <c r="F19" s="60"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
         <v>43</v>
@@ -4855,31 +4873,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="56" t="s">
+      <c r="G21" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56" t="s">
+      <c r="H21" s="57"/>
+      <c r="I21" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="56"/>
+      <c r="J21" s="57"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
@@ -4889,14 +4907,14 @@
         <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="56" t="s">
+      <c r="G22" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56" t="s">
+      <c r="H22" s="57"/>
+      <c r="I22" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="56"/>
+      <c r="J22" s="57"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
@@ -4906,14 +4924,14 @@
         <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="56" t="s">
+      <c r="G23" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56">
+      <c r="H23" s="57"/>
+      <c r="I23" s="57">
         <v>9</v>
       </c>
-      <c r="J23" s="56"/>
+      <c r="J23" s="57"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -4949,92 +4967,116 @@
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="57" t="s">
+      <c r="G31" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="57"/>
+      <c r="H31" s="56"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="53">
+      <c r="G32" s="54">
         <f>F32-G18</f>
         <v>43</v>
       </c>
-      <c r="H32" s="54"/>
+      <c r="H32" s="55"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="53">
+      <c r="G33" s="54">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="54"/>
+      <c r="H33" s="55"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="53">
+      <c r="G34" s="54">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="54"/>
+      <c r="H34" s="55"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="53">
+      <c r="G35" s="54">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="54"/>
+      <c r="H35" s="55"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="53">
+      <c r="G36" s="54">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="54"/>
+      <c r="H36" s="55"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="53">
+      <c r="G37" s="54">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="54"/>
+      <c r="H37" s="55"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="53">
+      <c r="G38" s="54">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="54"/>
+      <c r="H38" s="55"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="53">
+      <c r="G39" s="54">
         <f>G38-N18</f>
         <v>8</v>
       </c>
-      <c r="H39" s="54"/>
+      <c r="H39" s="55"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="53">
+      <c r="G40" s="54">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="54"/>
+      <c r="H40" s="55"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="36">
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G20:O20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C12:D12"/>
@@ -5047,30 +5089,6 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -5104,28 +5122,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
       <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="31" t="s">
         <v>55</v>
       </c>
@@ -5159,10 +5177,10 @@
     </row>
     <row r="5" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="25"/>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="58"/>
+      <c r="E5" s="53"/>
       <c r="F5" s="21" t="s">
         <v>34</v>
       </c>
@@ -5325,10 +5343,10 @@
       <c r="C9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="54"/>
+      <c r="E9" s="55"/>
       <c r="F9" s="20">
         <v>4</v>
       </c>
@@ -5361,7 +5379,7 @@
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="62" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="23"/>
@@ -5404,7 +5422,7 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="60"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
         <v>64</v>
@@ -5441,11 +5459,11 @@
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="61"/>
-      <c r="D12" s="53" t="s">
+      <c r="C12" s="64"/>
+      <c r="D12" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="54"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="20">
         <v>2</v>
       </c>
@@ -5482,13 +5500,13 @@
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="54"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="20">
         <v>4</v>
       </c>
@@ -5521,11 +5539,11 @@
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="60"/>
-      <c r="D14" s="53" t="s">
+      <c r="C14" s="63"/>
+      <c r="D14" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="54"/>
+      <c r="E14" s="55"/>
       <c r="F14" s="20">
         <v>6</v>
       </c>
@@ -5564,11 +5582,11 @@
       </c>
     </row>
     <row r="15" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="61"/>
-      <c r="D15" s="53" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="54"/>
+      <c r="E15" s="55"/>
       <c r="F15" s="20">
         <v>2</v>
       </c>
@@ -5691,7 +5709,7 @@
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="62" t="s">
         <v>69</v>
       </c>
       <c r="D18" s="52" t="s">
@@ -5728,11 +5746,11 @@
       <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="60"/>
-      <c r="D19" s="53" t="s">
+      <c r="C19" s="63"/>
+      <c r="D19" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="54"/>
+      <c r="E19" s="55"/>
       <c r="F19" s="20">
         <v>8</v>
       </c>
@@ -5769,7 +5787,7 @@
       <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="61"/>
+      <c r="C20" s="64"/>
       <c r="D20" s="52" t="s">
         <v>21</v>
       </c>
@@ -5810,7 +5828,7 @@
       <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="55"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
         <v>23</v>
@@ -5819,7 +5837,7 @@
         <f>SUM(F6:F20)</f>
         <v>62</v>
       </c>
-      <c r="G21" s="55"/>
+      <c r="G21" s="60"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -5832,13 +5850,13 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="50"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="55"/>
+      <c r="G22" s="60"/>
       <c r="H22" s="8">
         <v>0</v>
       </c>
@@ -5872,7 +5890,7 @@
       </c>
     </row>
     <row r="23" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="50"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>36</v>
@@ -5881,7 +5899,7 @@
         <f>F21</f>
         <v>62</v>
       </c>
-      <c r="G23" s="55"/>
+      <c r="G23" s="60"/>
       <c r="H23" s="8">
         <f>F23-H22</f>
         <v>62</v>
@@ -5927,14 +5945,14 @@
       <c r="F28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="62" t="s">
+      <c r="I28" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62" t="s">
+      <c r="J28" s="61"/>
+      <c r="K28" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="L28" s="62"/>
+      <c r="L28" s="61"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E29" s="3" t="s">
@@ -5944,14 +5962,14 @@
         <f>SUM(F18:F20)</f>
         <v>15</v>
       </c>
-      <c r="I29" s="62" t="s">
+      <c r="I29" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62" t="s">
+      <c r="J29" s="61"/>
+      <c r="K29" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="62"/>
+      <c r="L29" s="61"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E30" s="3" t="s">
@@ -5961,14 +5979,14 @@
         <f>SUM(F6:F8)</f>
         <v>16</v>
       </c>
-      <c r="I30" s="62" t="s">
+      <c r="I30" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="62"/>
-      <c r="K30" s="62">
+      <c r="J30" s="61"/>
+      <c r="K30" s="61">
         <v>10</v>
       </c>
-      <c r="L30" s="62"/>
+      <c r="L30" s="61"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
@@ -6082,14 +6100,12 @@
   </sheetData>
   <autoFilter ref="E39:F49"/>
   <mergeCells count="25">
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="D20:E20"/>
@@ -6101,12 +6117,14 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6116,10 +6134,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:R41"/>
+  <dimension ref="C4:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6141,11 +6159,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="47"/>
       <c r="J4" s="47"/>
       <c r="K4" s="47"/>
@@ -6158,11 +6176,11 @@
       <c r="R4" s="42"/>
     </row>
     <row r="5" spans="4:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
       <c r="I5" s="31" t="s">
         <v>97</v>
       </c>
@@ -6189,10 +6207,10 @@
     </row>
     <row r="6" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D6" s="44"/>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="58"/>
+      <c r="F6" s="53"/>
       <c r="G6" s="43" t="s">
         <v>34</v>
       </c>
@@ -6327,15 +6345,15 @@
     </row>
     <row r="10" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D10" s="46"/>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="54"/>
+      <c r="F10" s="55"/>
       <c r="G10" s="41">
         <v>2</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
@@ -6346,13 +6364,13 @@
       <c r="O10" s="41"/>
     </row>
     <row r="11" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="54"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="41">
         <v>2</v>
       </c>
@@ -6382,11 +6400,11 @@
       </c>
     </row>
     <row r="12" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="60"/>
-      <c r="E12" s="53" t="s">
+      <c r="D12" s="63"/>
+      <c r="E12" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="F12" s="54"/>
+      <c r="F12" s="55"/>
       <c r="G12" s="41">
         <v>5</v>
       </c>
@@ -6402,16 +6420,16 @@
       <c r="O12" s="36"/>
     </row>
     <row r="13" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="61"/>
-      <c r="E13" s="53" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="F13" s="54"/>
+      <c r="F13" s="55"/>
       <c r="G13" s="41">
         <v>2</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
@@ -6421,423 +6439,488 @@
       <c r="N13" s="41"/>
       <c r="O13" s="36"/>
     </row>
-    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D14" s="59" t="s">
+    <row r="14" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="50"/>
+      <c r="E14" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="55"/>
+      <c r="G14" s="49">
+        <v>3</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="55"/>
+      <c r="G15" s="49">
+        <v>3</v>
+      </c>
+      <c r="H15" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="36"/>
+    </row>
+    <row r="16" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="50"/>
+      <c r="E16" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="55"/>
+      <c r="G16" s="49">
+        <v>2</v>
+      </c>
+      <c r="H16" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="36"/>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D17" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E17" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="41">
-        <v>2</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="41">
-        <v>4</v>
-      </c>
-      <c r="J14" s="41">
-        <v>4</v>
-      </c>
-      <c r="K14" s="41">
-        <v>4</v>
-      </c>
-      <c r="L14" s="41">
-        <v>4</v>
-      </c>
-      <c r="M14" s="41">
-        <v>4</v>
-      </c>
-      <c r="N14" s="41">
-        <v>4</v>
-      </c>
-      <c r="O14" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D15" s="60"/>
-      <c r="E15" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="54"/>
-      <c r="G15" s="41">
-        <v>3</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="41">
-        <v>2</v>
-      </c>
-      <c r="J15" s="41">
-        <v>2</v>
-      </c>
-      <c r="K15" s="41">
-        <v>2</v>
-      </c>
-      <c r="L15" s="41">
-        <v>2</v>
-      </c>
-      <c r="M15" s="41">
-        <v>2</v>
-      </c>
-      <c r="N15" s="41">
-        <v>2</v>
-      </c>
-      <c r="O15" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D16" s="60"/>
-      <c r="E16" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="41">
-        <v>2</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="36"/>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="60"/>
-      <c r="E17" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="54"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="36"/>
+      <c r="I17" s="41">
+        <v>4</v>
+      </c>
+      <c r="J17" s="41">
+        <v>4</v>
+      </c>
+      <c r="K17" s="41">
+        <v>4</v>
+      </c>
+      <c r="L17" s="41">
+        <v>4</v>
+      </c>
+      <c r="M17" s="41">
+        <v>4</v>
+      </c>
+      <c r="N17" s="41">
+        <v>4</v>
+      </c>
+      <c r="O17" s="41">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="60"/>
-      <c r="E18" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="54"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="55"/>
       <c r="G18" s="41">
         <v>3</v>
       </c>
       <c r="H18" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="36"/>
+      <c r="I18" s="41">
+        <v>2</v>
+      </c>
+      <c r="J18" s="41">
+        <v>2</v>
+      </c>
+      <c r="K18" s="41">
+        <v>2</v>
+      </c>
+      <c r="L18" s="41">
+        <v>2</v>
+      </c>
+      <c r="M18" s="41">
+        <v>2</v>
+      </c>
+      <c r="N18" s="41">
+        <v>2</v>
+      </c>
+      <c r="O18" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="61"/>
-      <c r="E19" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="54"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="55"/>
       <c r="G19" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="41">
-        <v>2</v>
-      </c>
-      <c r="J19" s="41">
-        <v>2</v>
-      </c>
-      <c r="K19" s="41">
-        <v>2</v>
-      </c>
-      <c r="L19" s="41">
-        <v>2</v>
-      </c>
-      <c r="M19" s="41">
-        <v>2</v>
-      </c>
-      <c r="N19" s="41">
-        <v>2</v>
-      </c>
-      <c r="O19" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D20" s="55"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5" t="s">
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="36"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="63"/>
+      <c r="E20" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="55"/>
+      <c r="G20" s="41">
+        <v>3</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="36"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D21" s="63"/>
+      <c r="E21" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="55"/>
+      <c r="G21" s="41">
+        <v>3</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="36"/>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D22" s="64"/>
+      <c r="E22" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="55"/>
+      <c r="G22" s="41">
+        <v>3</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="41">
+        <v>2</v>
+      </c>
+      <c r="J22" s="41">
+        <v>2</v>
+      </c>
+      <c r="K22" s="41">
+        <v>2</v>
+      </c>
+      <c r="L22" s="41">
+        <v>2</v>
+      </c>
+      <c r="M22" s="41">
+        <v>2</v>
+      </c>
+      <c r="N22" s="41">
+        <v>2</v>
+      </c>
+      <c r="O22" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="60"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="8">
-        <f>SUM(G7:G19)</f>
-        <v>34</v>
-      </c>
-      <c r="H20" s="55"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D21" s="50"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5" t="s">
+      <c r="G23" s="8">
+        <f>SUM(G7:G22)</f>
+        <v>42</v>
+      </c>
+      <c r="H23" s="60"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D24" s="51"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="8">
-        <v>2</v>
-      </c>
-      <c r="J21" s="8">
+      <c r="G24" s="8"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="8">
+        <v>2</v>
+      </c>
+      <c r="J24" s="8">
         <v>3</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K24" s="8">
         <v>4</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L24" s="8">
         <v>5</v>
       </c>
-      <c r="M21" s="8">
+      <c r="M24" s="8">
         <v>4</v>
       </c>
-      <c r="N21" s="8">
+      <c r="N24" s="8">
         <v>3</v>
       </c>
-      <c r="O21" s="8">
+      <c r="O24" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D22" s="50"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5" t="s">
+    <row r="25" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="51"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="8">
-        <f>G20</f>
-        <v>34</v>
-      </c>
-      <c r="H22" s="55"/>
-      <c r="I22" s="8">
-        <f>G22-I21</f>
+      <c r="G25" s="8">
+        <f>G23</f>
+        <v>42</v>
+      </c>
+      <c r="H25" s="60"/>
+      <c r="I25" s="8">
+        <f>G25-I24</f>
+        <v>40</v>
+      </c>
+      <c r="J25" s="8">
+        <f>I25-J24</f>
+        <v>37</v>
+      </c>
+      <c r="K25" s="8">
+        <f t="shared" ref="K25:L25" si="0">J25-K24</f>
+        <v>33</v>
+      </c>
+      <c r="L25" s="8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="M25" s="8">
+        <f>L25-M24</f>
+        <v>24</v>
+      </c>
+      <c r="N25" s="8">
+        <f>M25-N24</f>
+        <v>21</v>
+      </c>
+      <c r="O25" s="8">
+        <f>N25-O24</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F30" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30" s="61"/>
+      <c r="M30" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F31" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="8">
-        <f>I22-J21</f>
-        <v>29</v>
-      </c>
-      <c r="K22" s="8">
-        <f t="shared" ref="K22:L22" si="0">J22-K21</f>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="I31" s="61"/>
+      <c r="L31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="4">
+        <f>SUM(G14:G16)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F32" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61">
+        <v>7</v>
+      </c>
+      <c r="I32" s="61"/>
+      <c r="L32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L22" s="8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M22" s="8">
-        <f>L22-M21</f>
+      <c r="M32" s="4">
+        <f>SUM(G7:G10)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="4">
+        <f>SUM(G17:G22)</f>
         <v>16</v>
       </c>
-      <c r="N22" s="8">
-        <f>M22-N21</f>
-        <v>13</v>
-      </c>
-      <c r="O22" s="8">
-        <f>N22-O21</f>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F27" s="62" t="s">
-        <v>104</v>
-      </c>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="I27" s="62"/>
-      <c r="M27" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F28" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="I28" s="62"/>
-      <c r="L28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" s="4">
-        <f>SUM(G10,G13,G16)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F29" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62">
-        <v>7</v>
-      </c>
-      <c r="I29" s="62"/>
-      <c r="L29" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M29" s="4">
-        <f>SUM(G7:G9)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="L30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M30" s="4">
-        <f>SUM(G14:G15,G17:G19)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="L31" s="3" t="s">
+    </row>
+    <row r="34" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M31" s="4">
-        <f>SUM(G11:G12)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L32" s="9" t="s">
+      <c r="M34" s="4">
+        <f>SUM(G11:G13)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M32" s="9">
-        <f>SUM(M28:M31)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F34" s="39" t="s">
+      <c r="M35" s="9">
+        <f>SUM(M31:M34)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F37" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G37" s="39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F35" s="40">
-        <f>G20</f>
-        <v>34</v>
-      </c>
-      <c r="G35" s="40">
-        <f>F35-I21</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F36" s="40"/>
-      <c r="G36" s="40">
-        <f>G35-J21</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F37" s="40"/>
-      <c r="G37" s="40">
-        <f>J22-K21</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F38" s="40"/>
+    <row r="38" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F38" s="40">
+        <f>G23</f>
+        <v>42</v>
+      </c>
       <c r="G38" s="40">
-        <f>K22-L21</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
+        <f>F38-I24</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F39" s="40"/>
       <c r="G39" s="40">
-        <f>G38-M21</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
+        <f>G38-J24</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F40" s="40"/>
       <c r="G40" s="40">
-        <f>G39-N21</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="6:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F41" s="40">
+        <f>J25-K24</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F41" s="40"/>
+      <c r="G41" s="40">
+        <f>K25-L24</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F42" s="40"/>
+      <c r="G42" s="40">
+        <f>G41-M24</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F43" s="40"/>
+      <c r="G43" s="40">
+        <f>G42-N24</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F44" s="40">
         <v>0</v>
       </c>
-      <c r="G41" s="40">
-        <f>G40-O21</f>
-        <v>-3</v>
+      <c r="G44" s="40">
+        <f>G43-O24</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F34:G41"/>
-  <mergeCells count="25">
+  <autoFilter ref="F37:G44"/>
+  <mergeCells count="28">
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="D4:H5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
U projektnu dokumentaciju dodan je opis sprintbacklog-a i opis burndowncharta zajedno sa slikom te su dodani opisi sastanaka i popravljeni plan iteracija.
</commit_message>
<xml_diff>
--- a/Dokumentacija/SprintBackLog.xlsx
+++ b/Dokumentacija/SprintBackLog.xlsx
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SpirntBacklog 2'!$E$39:$F$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SprintBackLog 1'!$F$31:$H$40</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SprintBacklog 3'!$F$37:$G$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SprintBacklog 3'!$F$38:$G$45</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="112">
   <si>
     <t>Zadatak</t>
   </si>
@@ -348,9 +348,6 @@
     <t>Početak 3.sprinta</t>
   </si>
   <si>
-    <t>24.01.2018.</t>
-  </si>
-  <si>
     <t>Izraditi dijagrame</t>
   </si>
   <si>
@@ -364,6 +361,12 @@
   </si>
   <si>
     <t>Analizirati i usporediti rezultate</t>
+  </si>
+  <si>
+    <t>25.01.2018.</t>
+  </si>
+  <si>
+    <t>Kreirati upute o lijeku</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -758,13 +761,22 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -773,22 +785,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -798,6 +804,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1097,11 +1112,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1718956016"/>
-        <c:axId val="1718956560"/>
+        <c:axId val="-1899523808"/>
+        <c:axId val="-1899522720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1718956016"/>
+        <c:axId val="-1899523808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,7 +1159,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1718956560"/>
+        <c:crossAx val="-1899522720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1152,7 +1167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1718956560"/>
+        <c:axId val="-1899522720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1218,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1718956016"/>
+        <c:crossAx val="-1899523808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1322,6 +1337,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1571,11 +1587,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1718959280"/>
-        <c:axId val="1718962000"/>
+        <c:axId val="-1900270416"/>
+        <c:axId val="-1900262800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1718959280"/>
+        <c:axId val="-1900270416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +1634,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1718962000"/>
+        <c:crossAx val="-1900262800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1626,7 +1642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1718962000"/>
+        <c:axId val="-1900262800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,7 +1693,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1718959280"/>
+        <c:crossAx val="-1900270416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1691,6 +1707,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1778,7 +1795,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1817,7 +1834,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1844,7 +1861,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SprintBacklog 3'!$F$37</c:f>
+              <c:f>'SprintBacklog 3'!$F$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1854,17 +1871,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'SprintBacklog 3'!$I$5:$O$5</c:f>
@@ -1896,12 +1922,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SprintBacklog 3'!$F$38:$F$44</c:f>
+              <c:f>'SprintBacklog 3'!$F$39:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1916,7 +1942,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SprintBacklog 3'!$G$37</c:f>
+              <c:f>'SprintBacklog 3'!$G$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1926,17 +1952,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'SprintBacklog 3'!$I$5:$O$5</c:f>
@@ -1968,30 +2003,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SprintBacklog 3'!$G$38:$G$44</c:f>
+              <c:f>'SprintBacklog 3'!$G$39:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1999,19 +2034,20 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1722025152"/>
-        <c:axId val="1722033312"/>
+        <c:axId val="-1896642608"/>
+        <c:axId val="-1896642064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1722025152"/>
+        <c:axId val="-1896642608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2023,7 +2059,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -2054,7 +2090,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1722033312"/>
+        <c:crossAx val="-1896642064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2062,7 +2098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1722033312"/>
+        <c:axId val="-1896642064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2113,7 +2149,7 @@
             <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1722025152"/>
+        <c:crossAx val="-1896642608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3320,7 +3356,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3331,7 +3367,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -3344,7 +3380,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -3361,7 +3397,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3377,7 +3413,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -3421,45 +3457,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3471,31 +3497,29 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -3599,14 +3623,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -3696,20 +3714,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3722,6 +3740,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3753,7 +3782,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3762,14 +3791,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3823,14 +3851,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3911,13 +3933,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>386290</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>83608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>232833</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4219,27 +4241,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="15" t="s">
         <v>39</v>
       </c>
@@ -4270,10 +4292,10 @@
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
@@ -4310,10 +4332,10 @@
     </row>
     <row r="4" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="2">
         <v>4</v>
       </c>
@@ -4348,10 +4370,10 @@
     </row>
     <row r="5" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26"/>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="52"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="2">
         <v>2</v>
       </c>
@@ -4384,10 +4406,10 @@
       <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="52"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="2">
         <v>2</v>
       </c>
@@ -4418,10 +4440,10 @@
     </row>
     <row r="7" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -4444,10 +4466,10 @@
     </row>
     <row r="8" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="26"/>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="56"/>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -4472,10 +4494,10 @@
     </row>
     <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="52"/>
+      <c r="D9" s="56"/>
       <c r="E9" s="2">
         <v>4</v>
       </c>
@@ -4504,10 +4526,10 @@
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="52"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="2">
         <v>5</v>
       </c>
@@ -4544,10 +4566,10 @@
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="52"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="2">
         <v>2</v>
       </c>
@@ -4584,10 +4606,10 @@
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="52"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="2">
         <v>2</v>
       </c>
@@ -4624,10 +4646,10 @@
     </row>
     <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28"/>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="52"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="2">
         <v>6</v>
       </c>
@@ -4662,10 +4684,10 @@
       <c r="B14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="52"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="12">
         <v>4</v>
       </c>
@@ -4692,10 +4714,10 @@
     </row>
     <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="29"/>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="55"/>
+      <c r="D15" s="58"/>
       <c r="E15" s="12">
         <v>5</v>
       </c>
@@ -4734,10 +4756,10 @@
       <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="52"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="12">
         <v>4</v>
       </c>
@@ -4769,7 +4791,7 @@
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="58"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
@@ -4778,7 +4800,7 @@
         <f>SUM(E4:E16)</f>
         <v>46</v>
       </c>
-      <c r="F17" s="58"/>
+      <c r="F17" s="53"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -4790,13 +4812,13 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="51"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="60"/>
+      <c r="F18" s="59"/>
       <c r="G18" s="8">
         <v>3</v>
       </c>
@@ -4826,7 +4848,7 @@
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="51"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -4834,7 +4856,7 @@
       <c r="E19" s="8">
         <v>46</v>
       </c>
-      <c r="F19" s="60"/>
+      <c r="F19" s="59"/>
       <c r="G19" s="8">
         <f>E19-G18</f>
         <v>43</v>
@@ -4873,31 +4895,31 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
       <c r="F20" s="19"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="57" t="s">
+      <c r="G21" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57" t="s">
+      <c r="H21" s="60"/>
+      <c r="I21" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="57"/>
+      <c r="J21" s="60"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
@@ -4907,14 +4929,14 @@
         <f>SUM(E4+E9+E14)</f>
         <v>12</v>
       </c>
-      <c r="G22" s="57" t="s">
+      <c r="G22" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57" t="s">
+      <c r="H22" s="60"/>
+      <c r="I22" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="57"/>
+      <c r="J22" s="60"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
@@ -4924,14 +4946,14 @@
         <f>SUM(E5+E7+E10+E12+E16)</f>
         <v>14</v>
       </c>
-      <c r="G23" s="57" t="s">
+      <c r="G23" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57">
+      <c r="H23" s="60"/>
+      <c r="I23" s="60">
         <v>9</v>
       </c>
-      <c r="J23" s="57"/>
+      <c r="J23" s="60"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -4967,116 +4989,92 @@
       <c r="F31" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="56" t="s">
+      <c r="G31" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="56"/>
+      <c r="H31" s="61"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" s="2">
         <v>46</v>
       </c>
-      <c r="G32" s="54">
+      <c r="G32" s="57">
         <f>F32-G18</f>
         <v>43</v>
       </c>
-      <c r="H32" s="55"/>
+      <c r="H32" s="58"/>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
-      <c r="G33" s="54">
+      <c r="G33" s="57">
         <f>G32-H18</f>
         <v>40</v>
       </c>
-      <c r="H33" s="55"/>
+      <c r="H33" s="58"/>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
-      <c r="G34" s="54">
+      <c r="G34" s="57">
         <f>G33-I18</f>
         <v>37</v>
       </c>
-      <c r="H34" s="55"/>
+      <c r="H34" s="58"/>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
-      <c r="G35" s="54">
+      <c r="G35" s="57">
         <f>G34-J18</f>
         <v>33</v>
       </c>
-      <c r="H35" s="55"/>
+      <c r="H35" s="58"/>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
-      <c r="G36" s="54">
+      <c r="G36" s="57">
         <f>G35-K18</f>
         <v>30</v>
       </c>
-      <c r="H36" s="55"/>
+      <c r="H36" s="58"/>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
-      <c r="G37" s="54">
+      <c r="G37" s="57">
         <f>G36-L18</f>
         <v>23</v>
       </c>
-      <c r="H37" s="55"/>
+      <c r="H37" s="58"/>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
-      <c r="G38" s="54">
+      <c r="G38" s="57">
         <f>G37-M18</f>
         <v>13</v>
       </c>
-      <c r="H38" s="55"/>
+      <c r="H38" s="58"/>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
-      <c r="G39" s="54">
+      <c r="G39" s="57">
         <f>G38-N18</f>
         <v>8</v>
       </c>
-      <c r="H39" s="55"/>
+      <c r="H39" s="58"/>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>0</v>
       </c>
-      <c r="G40" s="54">
+      <c r="G40" s="57">
         <f>G39-O18</f>
         <v>0</v>
       </c>
-      <c r="H40" s="55"/>
+      <c r="H40" s="58"/>
     </row>
   </sheetData>
   <autoFilter ref="F31:H40">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="36">
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
     <mergeCell ref="G20:O20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C12:D12"/>
@@ -5089,6 +5087,30 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -5100,7 +5122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Q49"/>
   <sheetViews>
-    <sheetView topLeftCell="E21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -5122,28 +5144,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
       <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="31" t="s">
         <v>55</v>
       </c>
@@ -5177,10 +5199,10 @@
     </row>
     <row r="5" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C5" s="25"/>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="53"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="21" t="s">
         <v>34</v>
       </c>
@@ -5220,10 +5242,10 @@
     </row>
     <row r="6" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C6" s="26"/>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="52"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="20">
         <v>9</v>
       </c>
@@ -5257,10 +5279,10 @@
     </row>
     <row r="7" spans="3:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C7" s="26"/>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="52"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="20">
         <v>5</v>
       </c>
@@ -5300,10 +5322,10 @@
       <c r="C8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="52"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="20">
         <v>2</v>
       </c>
@@ -5343,10 +5365,10 @@
       <c r="C9" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="55"/>
+      <c r="E9" s="58"/>
       <c r="F9" s="20">
         <v>4</v>
       </c>
@@ -5379,7 +5401,7 @@
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="63" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="23"/>
@@ -5422,7 +5444,7 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="63"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
         <v>64</v>
@@ -5459,11 +5481,11 @@
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="64"/>
-      <c r="D12" s="54" t="s">
+      <c r="C12" s="65"/>
+      <c r="D12" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="58"/>
       <c r="F12" s="20">
         <v>2</v>
       </c>
@@ -5500,13 +5522,13 @@
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="55"/>
+      <c r="E13" s="58"/>
       <c r="F13" s="20">
         <v>4</v>
       </c>
@@ -5539,11 +5561,11 @@
       <c r="Q13" s="20"/>
     </row>
     <row r="14" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="63"/>
-      <c r="D14" s="54" t="s">
+      <c r="C14" s="64"/>
+      <c r="D14" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="55"/>
+      <c r="E14" s="58"/>
       <c r="F14" s="20">
         <v>6</v>
       </c>
@@ -5582,11 +5604,11 @@
       </c>
     </row>
     <row r="15" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="64"/>
-      <c r="D15" s="54" t="s">
+      <c r="C15" s="65"/>
+      <c r="D15" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="55"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="20">
         <v>2</v>
       </c>
@@ -5709,13 +5731,13 @@
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="52"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="20">
         <v>5</v>
       </c>
@@ -5746,11 +5768,11 @@
       <c r="Q18" s="20"/>
     </row>
     <row r="19" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="63"/>
-      <c r="D19" s="54" t="s">
+      <c r="C19" s="64"/>
+      <c r="D19" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="55"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="20">
         <v>8</v>
       </c>
@@ -5787,11 +5809,11 @@
       <c r="Q19" s="20"/>
     </row>
     <row r="20" spans="3:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="64"/>
-      <c r="D20" s="52" t="s">
+      <c r="C20" s="65"/>
+      <c r="D20" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="52"/>
+      <c r="E20" s="56"/>
       <c r="F20" s="20">
         <v>2</v>
       </c>
@@ -5828,7 +5850,7 @@
       <c r="Q20" s="20"/>
     </row>
     <row r="21" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="60"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5" t="s">
         <v>23</v>
@@ -5837,7 +5859,7 @@
         <f>SUM(F6:F20)</f>
         <v>62</v>
       </c>
-      <c r="G21" s="60"/>
+      <c r="G21" s="59"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -5850,13 +5872,13 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="51"/>
+      <c r="C22" s="54"/>
       <c r="D22" s="7"/>
       <c r="E22" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="60"/>
+      <c r="G22" s="59"/>
       <c r="H22" s="8">
         <v>0</v>
       </c>
@@ -5890,7 +5912,7 @@
       </c>
     </row>
     <row r="23" spans="3:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="51"/>
+      <c r="C23" s="54"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>36</v>
@@ -5899,7 +5921,7 @@
         <f>F21</f>
         <v>62</v>
       </c>
-      <c r="G23" s="60"/>
+      <c r="G23" s="59"/>
       <c r="H23" s="8">
         <f>F23-H22</f>
         <v>62</v>
@@ -5945,14 +5967,14 @@
       <c r="F28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="61" t="s">
+      <c r="I28" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61" t="s">
+      <c r="J28" s="66"/>
+      <c r="K28" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="L28" s="61"/>
+      <c r="L28" s="66"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E29" s="3" t="s">
@@ -5962,14 +5984,14 @@
         <f>SUM(F18:F20)</f>
         <v>15</v>
       </c>
-      <c r="I29" s="61" t="s">
+      <c r="I29" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61" t="s">
+      <c r="J29" s="66"/>
+      <c r="K29" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="L29" s="61"/>
+      <c r="L29" s="66"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E30" s="3" t="s">
@@ -5979,14 +6001,14 @@
         <f>SUM(F6:F8)</f>
         <v>16</v>
       </c>
-      <c r="I30" s="61" t="s">
+      <c r="I30" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61">
+      <c r="J30" s="66"/>
+      <c r="K30" s="66">
         <v>10</v>
       </c>
-      <c r="L30" s="61"/>
+      <c r="L30" s="66"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
@@ -6100,12 +6122,14 @@
   </sheetData>
   <autoFilter ref="E39:F49"/>
   <mergeCells count="25">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:G4"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="D20:E20"/>
@@ -6117,14 +6141,12 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6134,10 +6156,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:R44"/>
+  <dimension ref="C4:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="D27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6159,11 +6181,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="47"/>
       <c r="J4" s="47"/>
       <c r="K4" s="47"/>
@@ -6176,11 +6198,11 @@
       <c r="R4" s="42"/>
     </row>
     <row r="5" spans="4:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
       <c r="I5" s="31" t="s">
         <v>97</v>
       </c>
@@ -6207,10 +6229,10 @@
     </row>
     <row r="6" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D6" s="44"/>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="53"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="43" t="s">
         <v>34</v>
       </c>
@@ -6241,10 +6263,10 @@
     </row>
     <row r="7" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D7" s="45"/>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="52"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="41">
         <v>1</v>
       </c>
@@ -6252,33 +6274,27 @@
         <v>25</v>
       </c>
       <c r="I7" s="41">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J7" s="41">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K7" s="41">
-        <v>9</v>
-      </c>
-      <c r="L7" s="13">
-        <v>9</v>
-      </c>
-      <c r="M7" s="41">
-        <v>9</v>
-      </c>
-      <c r="N7" s="41">
-        <v>4</v>
-      </c>
-      <c r="O7" s="36">
+        <v>1</v>
+      </c>
+      <c r="L7" s="67">
         <v>0</v>
       </c>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="68"/>
     </row>
     <row r="8" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D8" s="45"/>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="F8" s="52"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="41">
         <v>2</v>
       </c>
@@ -6286,35 +6302,33 @@
         <v>25</v>
       </c>
       <c r="I8" s="41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K8" s="41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L8" s="41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M8" s="41">
-        <v>3</v>
-      </c>
-      <c r="N8" s="35">
         <v>1</v>
       </c>
-      <c r="O8" s="41">
-        <v>1</v>
-      </c>
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="41"/>
     </row>
     <row r="9" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D9" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="52"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="41">
         <v>4</v>
       </c>
@@ -6322,229 +6336,297 @@
         <v>25</v>
       </c>
       <c r="I9" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J9" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K9" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L9" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M9" s="41">
         <v>2</v>
       </c>
-      <c r="N9" s="35">
-        <v>2</v>
-      </c>
-      <c r="O9" s="41">
-        <v>2</v>
-      </c>
+      <c r="N9" s="14">
+        <v>0</v>
+      </c>
+      <c r="O9" s="41"/>
     </row>
     <row r="10" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D10" s="46"/>
-      <c r="E10" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="41">
-        <v>2</v>
-      </c>
-      <c r="H10" s="41" t="s">
+      <c r="D10" s="52"/>
+      <c r="E10" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="51">
+        <v>4</v>
+      </c>
+      <c r="H10" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="41"/>
-    </row>
-    <row r="11" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="62" t="s">
+      <c r="I10" s="51">
+        <v>4</v>
+      </c>
+      <c r="J10" s="51">
+        <v>2</v>
+      </c>
+      <c r="K10" s="14">
+        <v>0</v>
+      </c>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="51"/>
+    </row>
+    <row r="11" spans="4:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D11" s="46"/>
+      <c r="E11" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="58"/>
+      <c r="G11" s="41">
+        <v>2</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="41">
+        <v>2</v>
+      </c>
+      <c r="J11" s="41">
+        <v>2</v>
+      </c>
+      <c r="K11" s="41">
+        <v>2</v>
+      </c>
+      <c r="L11" s="41">
+        <v>2</v>
+      </c>
+      <c r="M11" s="41">
+        <v>2</v>
+      </c>
+      <c r="N11" s="35">
+        <v>2</v>
+      </c>
+      <c r="O11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E12" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="41">
-        <v>2</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="41">
-        <v>4</v>
-      </c>
-      <c r="J11" s="41">
-        <v>4</v>
-      </c>
-      <c r="K11" s="41">
-        <v>4</v>
-      </c>
-      <c r="L11" s="35">
-        <v>4</v>
-      </c>
-      <c r="M11" s="41">
-        <v>4</v>
-      </c>
-      <c r="N11" s="41">
-        <v>3</v>
-      </c>
-      <c r="O11" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="63"/>
-      <c r="E12" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="55"/>
+      <c r="F12" s="58"/>
       <c r="G12" s="41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H12" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="36"/>
+      <c r="I12" s="41">
+        <v>2</v>
+      </c>
+      <c r="J12" s="41">
+        <v>2</v>
+      </c>
+      <c r="K12" s="41">
+        <v>2</v>
+      </c>
+      <c r="L12" s="35">
+        <v>2</v>
+      </c>
+      <c r="M12" s="41">
+        <v>2</v>
+      </c>
+      <c r="N12" s="14">
+        <v>0</v>
+      </c>
+      <c r="O12" s="68"/>
     </row>
     <row r="13" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="64"/>
-      <c r="E13" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="55"/>
+      <c r="E13" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="58"/>
       <c r="G13" s="41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H13" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="36"/>
-    </row>
-    <row r="14" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="50"/>
-      <c r="E14" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="49">
+      <c r="I13" s="41">
+        <v>5</v>
+      </c>
+      <c r="J13" s="41">
+        <v>5</v>
+      </c>
+      <c r="K13" s="41">
+        <v>5</v>
+      </c>
+      <c r="L13" s="35">
+        <v>5</v>
+      </c>
+      <c r="M13" s="41">
+        <v>5</v>
+      </c>
+      <c r="N13" s="41">
         <v>3</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="36"/>
+      <c r="O13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="65"/>
+      <c r="E14" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="58"/>
+      <c r="G14" s="41">
+        <v>2</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="41">
+        <v>2</v>
+      </c>
+      <c r="J14" s="41">
+        <v>2</v>
+      </c>
+      <c r="K14" s="41">
+        <v>2</v>
+      </c>
+      <c r="L14" s="35">
+        <v>2</v>
+      </c>
+      <c r="M14" s="41">
+        <v>2</v>
+      </c>
+      <c r="N14" s="41">
+        <v>2</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="50"/>
+      <c r="E15" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" s="55"/>
+      <c r="F15" s="58"/>
       <c r="G15" s="49">
         <v>3</v>
       </c>
       <c r="H15" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="36"/>
+      <c r="I15" s="49">
+        <v>3</v>
+      </c>
+      <c r="J15" s="49">
+        <v>3</v>
+      </c>
+      <c r="K15" s="49">
+        <v>3</v>
+      </c>
+      <c r="L15" s="35">
+        <v>3</v>
+      </c>
+      <c r="M15" s="49">
+        <v>2</v>
+      </c>
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="68"/>
     </row>
     <row r="16" spans="4:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="50"/>
-      <c r="E16" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="55"/>
+      <c r="D16" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" s="58"/>
       <c r="G16" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="36"/>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="62" t="s">
+      <c r="I16" s="49">
+        <v>3</v>
+      </c>
+      <c r="J16" s="49">
+        <v>3</v>
+      </c>
+      <c r="K16" s="49">
+        <v>3</v>
+      </c>
+      <c r="L16" s="35">
+        <v>3</v>
+      </c>
+      <c r="M16" s="49">
+        <v>3</v>
+      </c>
+      <c r="N16" s="14">
+        <v>0</v>
+      </c>
+      <c r="O16" s="68"/>
+    </row>
+    <row r="17" spans="4:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="50"/>
+      <c r="E17" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="58"/>
+      <c r="G17" s="49">
+        <v>2</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="49">
+        <v>2</v>
+      </c>
+      <c r="J17" s="49">
+        <v>2</v>
+      </c>
+      <c r="K17" s="49">
+        <v>2</v>
+      </c>
+      <c r="L17" s="35">
+        <v>2</v>
+      </c>
+      <c r="M17" s="49">
+        <v>2</v>
+      </c>
+      <c r="N17" s="49">
+        <v>2</v>
+      </c>
+      <c r="O17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D18" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="E18" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="41">
-        <v>2</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="41">
-        <v>4</v>
-      </c>
-      <c r="J17" s="41">
-        <v>4</v>
-      </c>
-      <c r="K17" s="41">
-        <v>4</v>
-      </c>
-      <c r="L17" s="41">
-        <v>4</v>
-      </c>
-      <c r="M17" s="41">
-        <v>4</v>
-      </c>
-      <c r="N17" s="41">
-        <v>4</v>
-      </c>
-      <c r="O17" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="63"/>
-      <c r="E18" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="F18" s="55"/>
+      <c r="F18" s="58"/>
       <c r="G18" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" s="41" t="s">
         <v>27</v>
@@ -6561,82 +6643,112 @@
       <c r="L18" s="41">
         <v>2</v>
       </c>
-      <c r="M18" s="41">
-        <v>2</v>
-      </c>
-      <c r="N18" s="41">
-        <v>2</v>
-      </c>
-      <c r="O18" s="36">
+      <c r="M18" s="14">
         <v>0</v>
       </c>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="63"/>
-      <c r="E19" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="F19" s="55"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="58"/>
       <c r="G19" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
+      <c r="I19" s="41">
+        <v>3</v>
+      </c>
+      <c r="J19" s="41">
+        <v>3</v>
+      </c>
+      <c r="K19" s="41">
+        <v>3</v>
+      </c>
+      <c r="L19" s="41">
+        <v>1</v>
+      </c>
+      <c r="M19" s="14">
+        <v>0</v>
+      </c>
       <c r="N19" s="41"/>
-      <c r="O19" s="36"/>
+      <c r="O19" s="68"/>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="63"/>
-      <c r="E20" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="55"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="58"/>
       <c r="G20" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="36"/>
+      <c r="I20" s="41">
+        <v>2</v>
+      </c>
+      <c r="J20" s="41">
+        <v>2</v>
+      </c>
+      <c r="K20" s="41">
+        <v>2</v>
+      </c>
+      <c r="L20" s="41">
+        <v>2</v>
+      </c>
+      <c r="M20" s="41">
+        <v>2</v>
+      </c>
+      <c r="N20" s="41">
+        <v>2</v>
+      </c>
+      <c r="O20" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D21" s="63"/>
-      <c r="E21" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="55"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="58"/>
       <c r="G21" s="41">
         <v>3</v>
       </c>
       <c r="H21" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
+      <c r="I21" s="41">
+        <v>3</v>
+      </c>
+      <c r="J21" s="41">
+        <v>3</v>
+      </c>
+      <c r="K21" s="41">
+        <v>3</v>
+      </c>
+      <c r="L21" s="41">
+        <v>3</v>
+      </c>
+      <c r="M21" s="41">
+        <v>0</v>
+      </c>
       <c r="N21" s="41"/>
-      <c r="O21" s="36"/>
+      <c r="O21" s="68"/>
     </row>
     <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D22" s="64"/>
-      <c r="E22" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="55"/>
+      <c r="E22" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="58"/>
       <c r="G22" s="41">
         <v>3</v>
       </c>
@@ -6644,283 +6756,316 @@
         <v>27</v>
       </c>
       <c r="I22" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J22" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K22" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L22" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M22" s="41">
-        <v>2</v>
-      </c>
-      <c r="N22" s="41">
-        <v>2</v>
-      </c>
-      <c r="O22" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D23" s="60"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="8">
-        <f>SUM(G7:G22)</f>
-        <v>42</v>
-      </c>
-      <c r="H23" s="60"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="N22" s="14">
+        <v>0</v>
+      </c>
+      <c r="O22" s="68"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D23" s="65"/>
+      <c r="E23" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="58"/>
+      <c r="G23" s="41">
+        <v>3</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="41">
+        <v>3</v>
+      </c>
+      <c r="J23" s="41">
+        <v>3</v>
+      </c>
+      <c r="K23" s="41">
+        <v>3</v>
+      </c>
+      <c r="L23" s="41">
+        <v>3</v>
+      </c>
+      <c r="M23" s="41">
+        <v>1</v>
+      </c>
+      <c r="N23" s="41">
+        <v>1</v>
+      </c>
+      <c r="O23" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D24" s="51"/>
+      <c r="D24" s="59"/>
       <c r="E24" s="7"/>
       <c r="F24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="8">
+        <f>SUM(G7:G23)</f>
+        <v>46</v>
+      </c>
+      <c r="H24" s="59"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="54"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="8">
-        <v>2</v>
-      </c>
-      <c r="J24" s="8">
+      <c r="G25" s="8"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="8">
+        <v>0</v>
+      </c>
+      <c r="J25" s="8">
+        <v>2</v>
+      </c>
+      <c r="K25" s="8">
+        <v>2</v>
+      </c>
+      <c r="L25" s="8">
         <v>3</v>
       </c>
-      <c r="K24" s="8">
-        <v>4</v>
-      </c>
-      <c r="L24" s="8">
-        <v>5</v>
-      </c>
-      <c r="M24" s="8">
-        <v>4</v>
-      </c>
-      <c r="N24" s="8">
-        <v>3</v>
-      </c>
-      <c r="O24" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D25" s="51"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5" t="s">
+      <c r="M25" s="8">
+        <v>14</v>
+      </c>
+      <c r="N25" s="8">
+        <v>13</v>
+      </c>
+      <c r="O25" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D26" s="54"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="8">
-        <f>G23</f>
+      <c r="G26" s="8">
+        <f>G24</f>
+        <v>46</v>
+      </c>
+      <c r="H26" s="59"/>
+      <c r="I26" s="8">
+        <f>G26-I25</f>
+        <v>46</v>
+      </c>
+      <c r="J26" s="8">
+        <f>I26-J25</f>
+        <v>44</v>
+      </c>
+      <c r="K26" s="8">
+        <f t="shared" ref="K26:L26" si="0">J26-K25</f>
         <v>42</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="8">
-        <f>G25-I24</f>
-        <v>40</v>
-      </c>
-      <c r="J25" s="8">
-        <f>I25-J24</f>
-        <v>37</v>
-      </c>
-      <c r="K25" s="8">
-        <f t="shared" ref="K25:L25" si="0">J25-K24</f>
+      <c r="L26" s="8">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="M26" s="8">
+        <f>L26-M25</f>
+        <v>25</v>
+      </c>
+      <c r="N26" s="8">
+        <f>M26-N25</f>
+        <v>12</v>
+      </c>
+      <c r="O26" s="8">
+        <f>N26-O25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F31" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="66"/>
+      <c r="M31" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F32" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="I32" s="66"/>
+      <c r="L32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" s="4">
+        <f>SUM(G15:G17)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F33" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="8">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="M25" s="8">
-        <f>L25-M24</f>
-        <v>24</v>
-      </c>
-      <c r="N25" s="8">
-        <f>M25-N24</f>
-        <v>21</v>
-      </c>
-      <c r="O25" s="8">
-        <f>N25-O24</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F30" s="61" t="s">
-        <v>104</v>
-      </c>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="I30" s="61"/>
-      <c r="M30" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F31" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="I31" s="61"/>
-      <c r="L31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" s="4">
-        <f>SUM(G14:G16)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F32" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61">
+      <c r="G33" s="66"/>
+      <c r="H33" s="66">
         <v>7</v>
       </c>
-      <c r="I32" s="61"/>
-      <c r="L32" s="3" t="s">
+      <c r="I33" s="66"/>
+      <c r="L33" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M32" s="4">
-        <f>SUM(G7:G10)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L33" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="M33" s="4">
-        <f>SUM(G17:G22)</f>
-        <v>16</v>
+        <f>SUM(G7:G11)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="6:13" x14ac:dyDescent="0.25">
       <c r="L34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" s="4">
+        <f>SUM(G18:G23)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L35" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M34" s="4">
-        <f>SUM(G11:G13)</f>
+      <c r="M35" s="4">
+        <f>SUM(G12:G14)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L35" s="9" t="s">
+    <row r="36" spans="6:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M35" s="9">
-        <f>SUM(M31:M34)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F37" s="39" t="s">
+      <c r="M36" s="9">
+        <f>SUM(M32:M35)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F38" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="39" t="s">
+      <c r="G38" s="39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F38" s="40">
-        <f>G23</f>
-        <v>42</v>
-      </c>
-      <c r="G38" s="40">
-        <f>F38-I24</f>
-        <v>40</v>
-      </c>
-    </row>
     <row r="39" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F39" s="40"/>
+      <c r="F39" s="40">
+        <f>G24</f>
+        <v>46</v>
+      </c>
       <c r="G39" s="40">
-        <f>G38-J24</f>
-        <v>37</v>
+        <f>F39-I25</f>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F40" s="40"/>
       <c r="G40" s="40">
-        <f>J25-K24</f>
-        <v>33</v>
+        <f>G39-J25</f>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F41" s="40"/>
       <c r="G41" s="40">
-        <f>K25-L24</f>
-        <v>28</v>
+        <f>J26-K25</f>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F42" s="40"/>
       <c r="G42" s="40">
-        <f>G41-M24</f>
-        <v>24</v>
+        <f>K26-L25</f>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F43" s="40"/>
       <c r="G43" s="40">
-        <f>G42-N24</f>
-        <v>21</v>
+        <f>G42-M25</f>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F44" s="40">
+      <c r="F44" s="40"/>
+      <c r="G44" s="40">
+        <f>G43-N25</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F45" s="40">
         <v>0</v>
       </c>
-      <c r="G44" s="40">
-        <f>G43-O24</f>
-        <v>5</v>
+      <c r="G45" s="40">
+        <f>G44-O25</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F37:G44"/>
-  <mergeCells count="28">
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
+  <autoFilter ref="F38:G45"/>
+  <mergeCells count="29">
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E20:F20"/>
     <mergeCell ref="D4:H5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>